<commit_message>
Added test data in the excel
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-sdutta2\ATaC_iCargo_WorkingDirectory\UiAutomationNew_2jan25\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alaskaair-my.sharepoint.com/personal/sourav_dutta2_alaskaair_com/Documents/Microsoft Teams Chat Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0C3910-2BA0-44CC-874C-AA439C66C1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{FA0C3910-2BA0-44CC-874C-AA439C66C1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E7FB2E9-7EF9-4470-A512-53E826D0742B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{16092AE6-4963-404B-A94C-F9A0B99B87F0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{16092AE6-4963-404B-A94C-F9A0B99B87F0}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LTE001_ACC_00001!$A$1:$Y$83</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="113">
   <si>
     <t>AgentCode</t>
   </si>
@@ -203,15 +206,6 @@
     <t>SAN</t>
   </si>
   <si>
-    <t>ORD</t>
-  </si>
-  <si>
-    <t>PHX</t>
-  </si>
-  <si>
-    <t>SFO</t>
-  </si>
-  <si>
     <t>LTE001_ACC_00005</t>
   </si>
   <si>
@@ -324,6 +318,66 @@
   </si>
   <si>
     <t>0666</t>
+  </si>
+  <si>
+    <t>DFW</t>
+  </si>
+  <si>
+    <t>UN2807</t>
+  </si>
+  <si>
+    <t>UN1977</t>
+  </si>
+  <si>
+    <t>UN1760</t>
+  </si>
+  <si>
+    <t>UN3373</t>
+  </si>
+  <si>
+    <t>UN1993</t>
+  </si>
+  <si>
+    <t>UN1324</t>
+  </si>
+  <si>
+    <t>UN3481</t>
+  </si>
+  <si>
+    <t>UN3287</t>
+  </si>
+  <si>
+    <t>UN1369</t>
+  </si>
+  <si>
+    <t>Magnetized material</t>
+  </si>
+  <si>
+    <t>Nitrogen, refrigerated liquid</t>
+  </si>
+  <si>
+    <t>Corrosive liquid n.o.s. *</t>
+  </si>
+  <si>
+    <t>Biological substance, Category B</t>
+  </si>
+  <si>
+    <t>Flammable liquid n.o.s. *</t>
+  </si>
+  <si>
+    <t>Films, nitrocellulose base</t>
+  </si>
+  <si>
+    <t>Y454</t>
+  </si>
+  <si>
+    <t>Lithium ion batteries contained in equipment</t>
+  </si>
+  <si>
+    <t>Toxic liquid, inorganic n.o.s. *</t>
+  </si>
+  <si>
+    <t>p-Nitrosodimethylaniline</t>
   </si>
 </sst>
 </file>
@@ -365,9 +419,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13A9B56-5E6E-4A35-9DD7-E48E0C4AA254}">
-  <dimension ref="A1:Y49"/>
+  <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T45" sqref="T45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -790,10 +847,10 @@
         <v>53</v>
       </c>
       <c r="V1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="W1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="X1" t="s">
         <v>15</v>
@@ -1347,7 +1404,7 @@
         <v>19</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J11" t="s">
         <v>19</v>
@@ -1453,7 +1510,7 @@
         <v>19</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J13" t="s">
         <v>19</v>
@@ -1494,13 +1551,13 @@
         <v>11377</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -1515,10 +1572,10 @@
         <v>19</v>
       </c>
       <c r="L14">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="M14">
-        <v>775</v>
+        <v>100</v>
       </c>
       <c r="N14" t="s">
         <v>32</v>
@@ -1533,7 +1590,7 @@
         <v>24</v>
       </c>
       <c r="Y14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.35">
@@ -1547,19 +1604,19 @@
         <v>11377</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
       </c>
-      <c r="I15">
-        <v>2199</v>
+      <c r="I15" t="s">
+        <v>20</v>
       </c>
       <c r="J15" t="s">
         <v>19</v>
@@ -1568,10 +1625,10 @@
         <v>19</v>
       </c>
       <c r="L15">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="M15">
-        <v>360</v>
+        <v>600</v>
       </c>
       <c r="N15" t="s">
         <v>32</v>
@@ -1586,7 +1643,7 @@
         <v>24</v>
       </c>
       <c r="Y15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.35">
@@ -1600,13 +1657,13 @@
         <v>11377</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H16" t="s">
         <v>19</v>
@@ -1621,10 +1678,10 @@
         <v>19</v>
       </c>
       <c r="L16">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="M16">
-        <v>150</v>
+        <v>750</v>
       </c>
       <c r="N16" t="s">
         <v>32</v>
@@ -1639,7 +1696,7 @@
         <v>24</v>
       </c>
       <c r="Y16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.35">
@@ -1653,13 +1710,13 @@
         <v>11377</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H17" t="s">
         <v>19</v>
@@ -1674,10 +1731,10 @@
         <v>19</v>
       </c>
       <c r="L17">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>1200</v>
+        <v>100</v>
       </c>
       <c r="N17" t="s">
         <v>32</v>
@@ -1692,7 +1749,7 @@
         <v>24</v>
       </c>
       <c r="Y17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.35">
@@ -1706,13 +1763,13 @@
         <v>11377</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="H18" t="s">
         <v>19</v>
@@ -1727,10 +1784,10 @@
         <v>19</v>
       </c>
       <c r="L18">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M18">
-        <v>14</v>
+        <v>600</v>
       </c>
       <c r="N18" t="s">
         <v>32</v>
@@ -1745,7 +1802,7 @@
         <v>24</v>
       </c>
       <c r="Y18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.35">
@@ -1759,19 +1816,19 @@
         <v>11377</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H19" t="s">
         <v>19</v>
       </c>
-      <c r="I19">
-        <v>2199</v>
+      <c r="I19" t="s">
+        <v>20</v>
       </c>
       <c r="J19" t="s">
         <v>19</v>
@@ -1780,10 +1837,10 @@
         <v>19</v>
       </c>
       <c r="L19">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="M19">
-        <v>775</v>
+        <v>750</v>
       </c>
       <c r="N19" t="s">
         <v>32</v>
@@ -1798,7 +1855,7 @@
         <v>24</v>
       </c>
       <c r="Y19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.35">
@@ -1851,7 +1908,7 @@
         <v>24</v>
       </c>
       <c r="Y20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.35">
@@ -1904,7 +1961,7 @@
         <v>24</v>
       </c>
       <c r="Y21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.35">
@@ -1960,7 +2017,7 @@
         <v>24</v>
       </c>
       <c r="Y22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.35">
@@ -2016,7 +2073,7 @@
         <v>24</v>
       </c>
       <c r="Y23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.35">
@@ -2069,7 +2126,7 @@
         <v>24</v>
       </c>
       <c r="Y24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.35">
@@ -2122,7 +2179,7 @@
         <v>24</v>
       </c>
       <c r="Y25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.35">
@@ -2175,7 +2232,7 @@
         <v>24</v>
       </c>
       <c r="Y26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.35">
@@ -2225,13 +2282,13 @@
         <v>23</v>
       </c>
       <c r="V27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="X27" t="s">
         <v>24</v>
       </c>
       <c r="Y27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.35">
@@ -2287,7 +2344,7 @@
         <v>24</v>
       </c>
       <c r="Y28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.35">
@@ -2301,7 +2358,7 @@
         <v>11377</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F29" t="s">
         <v>17</v>
@@ -2313,7 +2370,7 @@
         <v>19</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J29" t="s">
         <v>19</v>
@@ -2340,7 +2397,7 @@
         <v>24</v>
       </c>
       <c r="Y29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.35">
@@ -2354,7 +2411,7 @@
         <v>11377</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F30" t="s">
         <v>17</v>
@@ -2393,7 +2450,7 @@
         <v>24</v>
       </c>
       <c r="Y30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.35">
@@ -2407,7 +2464,7 @@
         <v>11377</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F31" t="s">
         <v>17</v>
@@ -2446,7 +2503,7 @@
         <v>24</v>
       </c>
       <c r="Y31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.35">
@@ -2499,7 +2556,7 @@
         <v>24</v>
       </c>
       <c r="Y32" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
@@ -2552,7 +2609,7 @@
         <v>24</v>
       </c>
       <c r="Y33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
@@ -2605,7 +2662,7 @@
         <v>24</v>
       </c>
       <c r="Y34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.35">
@@ -2628,13 +2685,13 @@
         <v>18</v>
       </c>
       <c r="H35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I35" t="s">
         <v>20</v>
       </c>
       <c r="J35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K35" t="s">
         <v>19</v>
@@ -2658,7 +2715,7 @@
         <v>1170</v>
       </c>
       <c r="R35" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S35">
         <v>364</v>
@@ -2673,7 +2730,7 @@
         <v>24</v>
       </c>
       <c r="Y35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.35">
@@ -2696,13 +2753,13 @@
         <v>18</v>
       </c>
       <c r="H36" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I36" t="s">
         <v>20</v>
       </c>
       <c r="J36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K36" t="s">
         <v>19</v>
@@ -2726,7 +2783,7 @@
         <v>3090</v>
       </c>
       <c r="R36" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="S36">
         <v>968</v>
@@ -2741,7 +2798,7 @@
         <v>24</v>
       </c>
       <c r="Y36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.35">
@@ -2764,13 +2821,13 @@
         <v>18</v>
       </c>
       <c r="H37" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" t="s">
         <v>69</v>
-      </c>
-      <c r="I37" t="s">
-        <v>20</v>
-      </c>
-      <c r="J37" t="s">
-        <v>72</v>
       </c>
       <c r="K37" t="s">
         <v>19</v>
@@ -2794,7 +2851,7 @@
         <v>1075</v>
       </c>
       <c r="R37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="S37">
         <v>200</v>
@@ -2809,7 +2866,7 @@
         <v>24</v>
       </c>
       <c r="Y37" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.35">
@@ -2829,10 +2886,10 @@
         <v>43</v>
       </c>
       <c r="G38" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H38" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I38" t="s">
         <v>20</v>
@@ -2862,7 +2919,7 @@
         <v>24</v>
       </c>
       <c r="Y38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.35">
@@ -2870,10 +2927,10 @@
         <v>27</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E39" t="s">
         <v>17</v>
@@ -2882,10 +2939,10 @@
         <v>37</v>
       </c>
       <c r="G39" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H39" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I39" t="s">
         <v>20</v>
@@ -2894,7 +2951,7 @@
         <v>19</v>
       </c>
       <c r="K39" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L39">
         <v>2</v>
@@ -2906,7 +2963,7 @@
         <v>21</v>
       </c>
       <c r="O39" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="P39" t="s">
         <v>23</v>
@@ -2915,7 +2972,7 @@
         <v>24</v>
       </c>
       <c r="Y39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">
@@ -2923,10 +2980,10 @@
         <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E40" t="s">
         <v>54</v>
@@ -2935,10 +2992,10 @@
         <v>31</v>
       </c>
       <c r="G40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I40" t="s">
         <v>20</v>
@@ -2947,7 +3004,7 @@
         <v>19</v>
       </c>
       <c r="K40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L40">
         <v>2</v>
@@ -2959,7 +3016,7 @@
         <v>21</v>
       </c>
       <c r="O40" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="P40" t="s">
         <v>23</v>
@@ -2968,7 +3025,7 @@
         <v>24</v>
       </c>
       <c r="Y40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.35">
@@ -2991,7 +3048,7 @@
         <v>33</v>
       </c>
       <c r="H41" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I41" t="s">
         <v>20</v>
@@ -3021,7 +3078,7 @@
         <v>24</v>
       </c>
       <c r="Y41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.35">
@@ -3071,13 +3128,13 @@
         <v>23</v>
       </c>
       <c r="V42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="X42" t="s">
         <v>24</v>
       </c>
       <c r="Y42" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.35">
@@ -3133,7 +3190,7 @@
         <v>24</v>
       </c>
       <c r="Y43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.35">
@@ -3186,7 +3243,7 @@
         <v>24</v>
       </c>
       <c r="Y44" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.35">
@@ -3200,7 +3257,7 @@
         <v>10763</v>
       </c>
       <c r="E45" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F45" t="s">
         <v>43</v>
@@ -3239,7 +3296,7 @@
         <v>24</v>
       </c>
       <c r="Y45" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.35">
@@ -3253,7 +3310,7 @@
         <v>10763</v>
       </c>
       <c r="E46" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F46" t="s">
         <v>43</v>
@@ -3292,7 +3349,7 @@
         <v>24</v>
       </c>
       <c r="Y46" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.35">
@@ -3306,7 +3363,7 @@
         <v>10763</v>
       </c>
       <c r="E47" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F47" t="s">
         <v>43</v>
@@ -3345,7 +3402,7 @@
         <v>24</v>
       </c>
       <c r="Y47" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.35">
@@ -3362,7 +3419,7 @@
         <v>17</v>
       </c>
       <c r="F48" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G48" t="s">
         <v>25</v>
@@ -3401,7 +3458,7 @@
         <v>24</v>
       </c>
       <c r="Y48" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.35">
@@ -3457,7 +3514,2079 @@
         <v>24</v>
       </c>
       <c r="Y49" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>11377</v>
+      </c>
+      <c r="C50">
+        <v>11377</v>
+      </c>
+      <c r="D50">
+        <v>11377</v>
+      </c>
+      <c r="E50" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" t="s">
+        <v>17</v>
+      </c>
+      <c r="G50" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>100</v>
+      </c>
+      <c r="N50" t="s">
+        <v>21</v>
+      </c>
+      <c r="O50" t="s">
+        <v>22</v>
+      </c>
+      <c r="P50" t="s">
+        <v>23</v>
+      </c>
+      <c r="X50" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>11377</v>
+      </c>
+      <c r="C51">
+        <v>11377</v>
+      </c>
+      <c r="D51">
+        <v>11377</v>
+      </c>
+      <c r="E51" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" t="s">
+        <v>17</v>
+      </c>
+      <c r="G51" t="s">
+        <v>33</v>
+      </c>
+      <c r="H51" t="s">
+        <v>19</v>
+      </c>
+      <c r="I51" t="s">
+        <v>20</v>
+      </c>
+      <c r="J51" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" t="s">
+        <v>19</v>
+      </c>
+      <c r="L51">
+        <v>8</v>
+      </c>
+      <c r="M51">
+        <v>600</v>
+      </c>
+      <c r="N51" t="s">
+        <v>21</v>
+      </c>
+      <c r="O51" t="s">
+        <v>22</v>
+      </c>
+      <c r="P51" t="s">
+        <v>23</v>
+      </c>
+      <c r="X51" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>11377</v>
+      </c>
+      <c r="C52">
+        <v>11377</v>
+      </c>
+      <c r="D52">
+        <v>11377</v>
+      </c>
+      <c r="E52" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" t="s">
+        <v>17</v>
+      </c>
+      <c r="G52" t="s">
+        <v>25</v>
+      </c>
+      <c r="H52" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" t="s">
+        <v>20</v>
+      </c>
+      <c r="J52" t="s">
+        <v>19</v>
+      </c>
+      <c r="K52" t="s">
+        <v>19</v>
+      </c>
+      <c r="L52">
+        <v>20</v>
+      </c>
+      <c r="M52">
+        <v>750</v>
+      </c>
+      <c r="N52" t="s">
+        <v>21</v>
+      </c>
+      <c r="O52" t="s">
+        <v>22</v>
+      </c>
+      <c r="P52" t="s">
+        <v>23</v>
+      </c>
+      <c r="X52" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53">
+        <v>10763</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" t="s">
+        <v>19</v>
+      </c>
+      <c r="I53" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" t="s">
+        <v>19</v>
+      </c>
+      <c r="L53">
+        <v>13</v>
+      </c>
+      <c r="M53">
+        <v>775</v>
+      </c>
+      <c r="N53" t="s">
+        <v>32</v>
+      </c>
+      <c r="O53" t="s">
+        <v>19</v>
+      </c>
+      <c r="P53" t="s">
+        <v>23</v>
+      </c>
+      <c r="X53" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54">
+        <v>10763</v>
+      </c>
+      <c r="E54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F54" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" t="s">
+        <v>33</v>
+      </c>
+      <c r="H54" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" t="s">
+        <v>20</v>
+      </c>
+      <c r="J54" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" t="s">
+        <v>19</v>
+      </c>
+      <c r="L54">
+        <v>8</v>
+      </c>
+      <c r="M54">
+        <v>360</v>
+      </c>
+      <c r="N54" t="s">
+        <v>32</v>
+      </c>
+      <c r="O54" t="s">
+        <v>19</v>
+      </c>
+      <c r="P54" t="s">
+        <v>23</v>
+      </c>
+      <c r="X54" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55">
+        <v>10763</v>
+      </c>
+      <c r="E55" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" t="s">
+        <v>17</v>
+      </c>
+      <c r="G55" t="s">
+        <v>25</v>
+      </c>
+      <c r="H55" t="s">
+        <v>19</v>
+      </c>
+      <c r="I55" t="s">
+        <v>20</v>
+      </c>
+      <c r="J55" t="s">
+        <v>19</v>
+      </c>
+      <c r="K55" t="s">
+        <v>19</v>
+      </c>
+      <c r="L55">
+        <v>2</v>
+      </c>
+      <c r="M55">
+        <v>59</v>
+      </c>
+      <c r="N55" t="s">
+        <v>32</v>
+      </c>
+      <c r="O55" t="s">
+        <v>19</v>
+      </c>
+      <c r="P55" t="s">
+        <v>23</v>
+      </c>
+      <c r="X55" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56">
+        <v>10763</v>
+      </c>
+      <c r="E56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F56" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56" t="s">
+        <v>18</v>
+      </c>
+      <c r="H56" t="s">
+        <v>19</v>
+      </c>
+      <c r="I56" t="s">
+        <v>20</v>
+      </c>
+      <c r="J56" t="s">
+        <v>19</v>
+      </c>
+      <c r="K56" t="s">
+        <v>19</v>
+      </c>
+      <c r="L56">
+        <v>13</v>
+      </c>
+      <c r="M56">
+        <v>775</v>
+      </c>
+      <c r="N56" t="s">
+        <v>32</v>
+      </c>
+      <c r="O56" t="s">
+        <v>19</v>
+      </c>
+      <c r="P56" t="s">
+        <v>23</v>
+      </c>
+      <c r="X56" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57">
+        <v>10763</v>
+      </c>
+      <c r="E57" t="s">
+        <v>93</v>
+      </c>
+      <c r="F57" t="s">
+        <v>17</v>
+      </c>
+      <c r="G57" t="s">
+        <v>33</v>
+      </c>
+      <c r="H57" t="s">
+        <v>19</v>
+      </c>
+      <c r="I57" t="s">
+        <v>20</v>
+      </c>
+      <c r="J57" t="s">
+        <v>19</v>
+      </c>
+      <c r="K57" t="s">
+        <v>19</v>
+      </c>
+      <c r="L57">
+        <v>8</v>
+      </c>
+      <c r="M57">
+        <v>360</v>
+      </c>
+      <c r="N57" t="s">
+        <v>32</v>
+      </c>
+      <c r="O57" t="s">
+        <v>19</v>
+      </c>
+      <c r="P57" t="s">
+        <v>23</v>
+      </c>
+      <c r="X57" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58">
+        <v>10763</v>
+      </c>
+      <c r="E58" t="s">
+        <v>87</v>
+      </c>
+      <c r="F58" t="s">
+        <v>17</v>
+      </c>
+      <c r="G58" t="s">
+        <v>25</v>
+      </c>
+      <c r="H58" t="s">
+        <v>19</v>
+      </c>
+      <c r="I58" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58" t="s">
+        <v>19</v>
+      </c>
+      <c r="K58" t="s">
+        <v>19</v>
+      </c>
+      <c r="L58">
+        <v>2</v>
+      </c>
+      <c r="M58">
+        <v>59</v>
+      </c>
+      <c r="N58" t="s">
+        <v>32</v>
+      </c>
+      <c r="O58" t="s">
+        <v>19</v>
+      </c>
+      <c r="P58" t="s">
+        <v>23</v>
+      </c>
+      <c r="X58" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>11377</v>
+      </c>
+      <c r="C59">
+        <v>11377</v>
+      </c>
+      <c r="D59">
+        <v>11377</v>
+      </c>
+      <c r="E59" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" t="s">
+        <v>37</v>
+      </c>
+      <c r="G59" t="s">
+        <v>18</v>
+      </c>
+      <c r="H59" t="s">
+        <v>38</v>
+      </c>
+      <c r="I59" t="s">
+        <v>20</v>
+      </c>
+      <c r="J59" t="s">
+        <v>94</v>
+      </c>
+      <c r="K59" t="s">
+        <v>19</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>30</v>
+      </c>
+      <c r="N59" t="s">
+        <v>32</v>
+      </c>
+      <c r="O59" t="s">
+        <v>19</v>
+      </c>
+      <c r="P59" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q59">
+        <v>2807</v>
+      </c>
+      <c r="R59" t="s">
+        <v>103</v>
+      </c>
+      <c r="S59" s="2">
+        <v>953</v>
+      </c>
+      <c r="T59">
+        <v>0.5</v>
+      </c>
+      <c r="U59" t="s">
+        <v>42</v>
+      </c>
+      <c r="X59" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>11377</v>
+      </c>
+      <c r="C60">
+        <v>11377</v>
+      </c>
+      <c r="D60">
+        <v>11377</v>
+      </c>
+      <c r="E60" t="s">
+        <v>54</v>
+      </c>
+      <c r="F60" t="s">
+        <v>31</v>
+      </c>
+      <c r="G60" t="s">
+        <v>18</v>
+      </c>
+      <c r="H60" t="s">
+        <v>38</v>
+      </c>
+      <c r="I60" t="s">
+        <v>20</v>
+      </c>
+      <c r="J60" t="s">
+        <v>95</v>
+      </c>
+      <c r="K60" t="s">
+        <v>19</v>
+      </c>
+      <c r="L60">
+        <v>2</v>
+      </c>
+      <c r="M60">
+        <v>65</v>
+      </c>
+      <c r="N60" t="s">
+        <v>32</v>
+      </c>
+      <c r="O60" t="s">
+        <v>19</v>
+      </c>
+      <c r="P60" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q60">
+        <v>1977</v>
+      </c>
+      <c r="R60" t="s">
+        <v>104</v>
+      </c>
+      <c r="S60">
+        <v>202</v>
+      </c>
+      <c r="T60">
+        <v>0.5</v>
+      </c>
+      <c r="U60" t="s">
+        <v>42</v>
+      </c>
+      <c r="X60" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>11377</v>
+      </c>
+      <c r="C61">
+        <v>11377</v>
+      </c>
+      <c r="D61">
+        <v>11377</v>
+      </c>
+      <c r="E61" t="s">
+        <v>54</v>
+      </c>
+      <c r="F61" t="s">
+        <v>31</v>
+      </c>
+      <c r="G61" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61" t="s">
+        <v>38</v>
+      </c>
+      <c r="I61" t="s">
+        <v>20</v>
+      </c>
+      <c r="J61" t="s">
+        <v>96</v>
+      </c>
+      <c r="K61" t="s">
+        <v>19</v>
+      </c>
+      <c r="L61">
+        <v>3</v>
+      </c>
+      <c r="M61">
+        <v>99</v>
+      </c>
+      <c r="N61" t="s">
+        <v>32</v>
+      </c>
+      <c r="O61" t="s">
+        <v>19</v>
+      </c>
+      <c r="P61" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q61">
+        <v>1760</v>
+      </c>
+      <c r="R61" t="s">
+        <v>105</v>
+      </c>
+      <c r="S61">
+        <v>850</v>
+      </c>
+      <c r="T61">
+        <v>0.5</v>
+      </c>
+      <c r="U61" t="s">
+        <v>42</v>
+      </c>
+      <c r="X61" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>11377</v>
+      </c>
+      <c r="C62">
+        <v>11377</v>
+      </c>
+      <c r="D62">
+        <v>11377</v>
+      </c>
+      <c r="E62" t="s">
+        <v>54</v>
+      </c>
+      <c r="F62" t="s">
+        <v>31</v>
+      </c>
+      <c r="G62" t="s">
+        <v>18</v>
+      </c>
+      <c r="H62" t="s">
+        <v>38</v>
+      </c>
+      <c r="I62" t="s">
+        <v>20</v>
+      </c>
+      <c r="J62" t="s">
+        <v>97</v>
+      </c>
+      <c r="K62" t="s">
+        <v>19</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+      <c r="M62">
+        <v>30</v>
+      </c>
+      <c r="N62" t="s">
+        <v>32</v>
+      </c>
+      <c r="O62" t="s">
+        <v>19</v>
+      </c>
+      <c r="P62" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q62">
+        <v>3373</v>
+      </c>
+      <c r="R62" t="s">
+        <v>106</v>
+      </c>
+      <c r="S62" s="2">
+        <v>650</v>
+      </c>
+      <c r="T62">
+        <v>0.5</v>
+      </c>
+      <c r="U62" t="s">
+        <v>42</v>
+      </c>
+      <c r="X62" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>11377</v>
+      </c>
+      <c r="C63">
+        <v>11377</v>
+      </c>
+      <c r="D63">
+        <v>11377</v>
+      </c>
+      <c r="E63" t="s">
+        <v>54</v>
+      </c>
+      <c r="F63" t="s">
+        <v>31</v>
+      </c>
+      <c r="G63" t="s">
+        <v>18</v>
+      </c>
+      <c r="H63" t="s">
+        <v>38</v>
+      </c>
+      <c r="I63" t="s">
+        <v>20</v>
+      </c>
+      <c r="J63" t="s">
+        <v>98</v>
+      </c>
+      <c r="K63" t="s">
+        <v>19</v>
+      </c>
+      <c r="L63">
+        <v>2</v>
+      </c>
+      <c r="M63">
+        <v>65</v>
+      </c>
+      <c r="N63" t="s">
+        <v>32</v>
+      </c>
+      <c r="O63" t="s">
+        <v>19</v>
+      </c>
+      <c r="P63" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q63">
+        <v>1993</v>
+      </c>
+      <c r="R63" t="s">
+        <v>107</v>
+      </c>
+      <c r="S63">
+        <v>351</v>
+      </c>
+      <c r="T63">
+        <v>0.5</v>
+      </c>
+      <c r="U63" t="s">
+        <v>42</v>
+      </c>
+      <c r="X63" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>11377</v>
+      </c>
+      <c r="C64">
+        <v>11377</v>
+      </c>
+      <c r="D64">
+        <v>11377</v>
+      </c>
+      <c r="E64" t="s">
+        <v>54</v>
+      </c>
+      <c r="F64" t="s">
+        <v>31</v>
+      </c>
+      <c r="G64" t="s">
+        <v>18</v>
+      </c>
+      <c r="H64" t="s">
+        <v>38</v>
+      </c>
+      <c r="I64" t="s">
+        <v>20</v>
+      </c>
+      <c r="J64" t="s">
+        <v>99</v>
+      </c>
+      <c r="K64" t="s">
+        <v>19</v>
+      </c>
+      <c r="L64">
+        <v>3</v>
+      </c>
+      <c r="M64">
+        <v>99</v>
+      </c>
+      <c r="N64" t="s">
+        <v>32</v>
+      </c>
+      <c r="O64" t="s">
+        <v>19</v>
+      </c>
+      <c r="P64" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q64">
+        <v>1324</v>
+      </c>
+      <c r="R64" t="s">
+        <v>108</v>
+      </c>
+      <c r="S64" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T64">
+        <v>0.5</v>
+      </c>
+      <c r="U64" t="s">
+        <v>42</v>
+      </c>
+      <c r="X64" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>11377</v>
+      </c>
+      <c r="C65">
+        <v>11377</v>
+      </c>
+      <c r="D65">
+        <v>11377</v>
+      </c>
+      <c r="E65" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" t="s">
+        <v>37</v>
+      </c>
+      <c r="G65" t="s">
+        <v>18</v>
+      </c>
+      <c r="H65" t="s">
+        <v>38</v>
+      </c>
+      <c r="I65" t="s">
+        <v>20</v>
+      </c>
+      <c r="J65" t="s">
+        <v>100</v>
+      </c>
+      <c r="K65" t="s">
+        <v>19</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+      <c r="M65">
+        <v>30</v>
+      </c>
+      <c r="N65" t="s">
+        <v>32</v>
+      </c>
+      <c r="O65" t="s">
+        <v>19</v>
+      </c>
+      <c r="P65" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q65">
+        <v>3481</v>
+      </c>
+      <c r="R65" t="s">
+        <v>110</v>
+      </c>
+      <c r="S65" s="2">
+        <v>967</v>
+      </c>
+      <c r="T65">
+        <v>0.5</v>
+      </c>
+      <c r="U65" t="s">
+        <v>42</v>
+      </c>
+      <c r="X65" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>11377</v>
+      </c>
+      <c r="C66">
+        <v>11377</v>
+      </c>
+      <c r="D66">
+        <v>11377</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" t="s">
+        <v>43</v>
+      </c>
+      <c r="G66" t="s">
+        <v>18</v>
+      </c>
+      <c r="H66" t="s">
+        <v>38</v>
+      </c>
+      <c r="I66" t="s">
+        <v>20</v>
+      </c>
+      <c r="J66" t="s">
+        <v>101</v>
+      </c>
+      <c r="K66" t="s">
+        <v>19</v>
+      </c>
+      <c r="L66">
+        <v>2</v>
+      </c>
+      <c r="M66">
+        <v>65</v>
+      </c>
+      <c r="N66" t="s">
+        <v>32</v>
+      </c>
+      <c r="O66" t="s">
+        <v>19</v>
+      </c>
+      <c r="P66" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q66">
+        <v>3287</v>
+      </c>
+      <c r="R66" t="s">
+        <v>111</v>
+      </c>
+      <c r="S66" s="2">
+        <v>652</v>
+      </c>
+      <c r="T66">
+        <v>0.5</v>
+      </c>
+      <c r="U66" t="s">
+        <v>42</v>
+      </c>
+      <c r="X66" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>11377</v>
+      </c>
+      <c r="C67">
+        <v>11377</v>
+      </c>
+      <c r="D67">
+        <v>11377</v>
+      </c>
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" t="s">
+        <v>46</v>
+      </c>
+      <c r="G67" t="s">
+        <v>18</v>
+      </c>
+      <c r="H67" t="s">
+        <v>38</v>
+      </c>
+      <c r="I67" t="s">
+        <v>20</v>
+      </c>
+      <c r="J67" t="s">
+        <v>102</v>
+      </c>
+      <c r="K67" t="s">
+        <v>19</v>
+      </c>
+      <c r="L67">
+        <v>3</v>
+      </c>
+      <c r="M67">
+        <v>99</v>
+      </c>
+      <c r="N67" t="s">
+        <v>32</v>
+      </c>
+      <c r="O67" t="s">
+        <v>19</v>
+      </c>
+      <c r="P67" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q67">
+        <v>1369</v>
+      </c>
+      <c r="R67" t="s">
+        <v>112</v>
+      </c>
+      <c r="S67" s="2">
+        <v>467</v>
+      </c>
+      <c r="T67">
+        <v>0.5</v>
+      </c>
+      <c r="U67" t="s">
+        <v>42</v>
+      </c>
+      <c r="X67" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>11377</v>
+      </c>
+      <c r="C68">
+        <v>11377</v>
+      </c>
+      <c r="D68">
+        <v>11377</v>
+      </c>
+      <c r="E68" t="s">
+        <v>93</v>
+      </c>
+      <c r="F68" t="s">
+        <v>17</v>
+      </c>
+      <c r="G68" t="s">
+        <v>18</v>
+      </c>
+      <c r="H68" t="s">
+        <v>38</v>
+      </c>
+      <c r="I68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J68" t="s">
+        <v>39</v>
+      </c>
+      <c r="K68" t="s">
+        <v>19</v>
+      </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
+      <c r="M68">
+        <v>30</v>
+      </c>
+      <c r="N68" t="s">
+        <v>21</v>
+      </c>
+      <c r="O68" t="s">
+        <v>22</v>
+      </c>
+      <c r="P68" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q68">
+        <v>8000</v>
+      </c>
+      <c r="R68" t="s">
+        <v>40</v>
+      </c>
+      <c r="S68" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T68">
+        <v>0.5</v>
+      </c>
+      <c r="U68" t="s">
+        <v>42</v>
+      </c>
+      <c r="X68" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>11377</v>
+      </c>
+      <c r="C69">
+        <v>11377</v>
+      </c>
+      <c r="D69">
+        <v>11377</v>
+      </c>
+      <c r="E69" t="s">
+        <v>93</v>
+      </c>
+      <c r="F69" t="s">
+        <v>17</v>
+      </c>
+      <c r="G69" t="s">
+        <v>18</v>
+      </c>
+      <c r="H69" t="s">
+        <v>38</v>
+      </c>
+      <c r="I69" t="s">
+        <v>20</v>
+      </c>
+      <c r="J69" t="s">
+        <v>44</v>
+      </c>
+      <c r="K69" t="s">
+        <v>19</v>
+      </c>
+      <c r="L69">
+        <v>2</v>
+      </c>
+      <c r="M69">
+        <v>65</v>
+      </c>
+      <c r="N69" t="s">
+        <v>21</v>
+      </c>
+      <c r="O69" t="s">
+        <v>22</v>
+      </c>
+      <c r="P69" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q69">
+        <v>1845</v>
+      </c>
+      <c r="R69" t="s">
+        <v>45</v>
+      </c>
+      <c r="S69">
+        <v>954</v>
+      </c>
+      <c r="T69">
+        <v>0.5</v>
+      </c>
+      <c r="U69" t="s">
+        <v>42</v>
+      </c>
+      <c r="X69" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>11377</v>
+      </c>
+      <c r="C70">
+        <v>11377</v>
+      </c>
+      <c r="D70">
+        <v>11377</v>
+      </c>
+      <c r="E70" t="s">
+        <v>93</v>
+      </c>
+      <c r="F70" t="s">
+        <v>17</v>
+      </c>
+      <c r="G70" t="s">
+        <v>18</v>
+      </c>
+      <c r="H70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I70" t="s">
+        <v>20</v>
+      </c>
+      <c r="J70" t="s">
+        <v>47</v>
+      </c>
+      <c r="K70" t="s">
+        <v>19</v>
+      </c>
+      <c r="L70">
+        <v>3</v>
+      </c>
+      <c r="M70">
+        <v>99</v>
+      </c>
+      <c r="N70" t="s">
+        <v>21</v>
+      </c>
+      <c r="O70" t="s">
+        <v>22</v>
+      </c>
+      <c r="P70" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q70">
+        <v>3110</v>
+      </c>
+      <c r="R70" t="s">
+        <v>48</v>
+      </c>
+      <c r="S70">
+        <v>570</v>
+      </c>
+      <c r="T70">
+        <v>0.5</v>
+      </c>
+      <c r="U70" t="s">
+        <v>42</v>
+      </c>
+      <c r="X70" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>11377</v>
+      </c>
+      <c r="C71">
+        <v>11377</v>
+      </c>
+      <c r="D71">
+        <v>11377</v>
+      </c>
+      <c r="E71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F71" t="s">
+        <v>17</v>
+      </c>
+      <c r="G71" t="s">
+        <v>18</v>
+      </c>
+      <c r="H71" t="s">
+        <v>38</v>
+      </c>
+      <c r="I71" t="s">
+        <v>20</v>
+      </c>
+      <c r="J71" t="s">
+        <v>94</v>
+      </c>
+      <c r="K71" t="s">
+        <v>19</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <v>30</v>
+      </c>
+      <c r="N71" t="s">
+        <v>32</v>
+      </c>
+      <c r="O71" t="s">
+        <v>19</v>
+      </c>
+      <c r="P71" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q71">
+        <v>2807</v>
+      </c>
+      <c r="R71" t="s">
+        <v>103</v>
+      </c>
+      <c r="S71" s="2">
+        <v>953</v>
+      </c>
+      <c r="T71">
+        <v>0.5</v>
+      </c>
+      <c r="U71" t="s">
+        <v>42</v>
+      </c>
+      <c r="X71" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>11377</v>
+      </c>
+      <c r="C72">
+        <v>11377</v>
+      </c>
+      <c r="D72">
+        <v>11377</v>
+      </c>
+      <c r="E72" t="s">
+        <v>93</v>
+      </c>
+      <c r="F72" t="s">
+        <v>17</v>
+      </c>
+      <c r="G72" t="s">
+        <v>18</v>
+      </c>
+      <c r="H72" t="s">
+        <v>38</v>
+      </c>
+      <c r="I72" t="s">
+        <v>20</v>
+      </c>
+      <c r="J72" t="s">
+        <v>95</v>
+      </c>
+      <c r="K72" t="s">
+        <v>19</v>
+      </c>
+      <c r="L72">
+        <v>2</v>
+      </c>
+      <c r="M72">
+        <v>65</v>
+      </c>
+      <c r="N72" t="s">
+        <v>32</v>
+      </c>
+      <c r="O72" t="s">
+        <v>19</v>
+      </c>
+      <c r="P72" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q72">
+        <v>1977</v>
+      </c>
+      <c r="R72" t="s">
+        <v>104</v>
+      </c>
+      <c r="S72">
+        <v>202</v>
+      </c>
+      <c r="T72">
+        <v>0.5</v>
+      </c>
+      <c r="U72" t="s">
+        <v>42</v>
+      </c>
+      <c r="X72" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>11377</v>
+      </c>
+      <c r="C73">
+        <v>11377</v>
+      </c>
+      <c r="D73">
+        <v>11377</v>
+      </c>
+      <c r="E73" t="s">
+        <v>93</v>
+      </c>
+      <c r="F73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G73" t="s">
+        <v>18</v>
+      </c>
+      <c r="H73" t="s">
+        <v>38</v>
+      </c>
+      <c r="I73" t="s">
+        <v>20</v>
+      </c>
+      <c r="J73" t="s">
+        <v>96</v>
+      </c>
+      <c r="K73" t="s">
+        <v>19</v>
+      </c>
+      <c r="L73">
+        <v>3</v>
+      </c>
+      <c r="M73">
+        <v>99</v>
+      </c>
+      <c r="N73" t="s">
+        <v>32</v>
+      </c>
+      <c r="O73" t="s">
+        <v>19</v>
+      </c>
+      <c r="P73" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q73">
+        <v>1760</v>
+      </c>
+      <c r="R73" t="s">
+        <v>105</v>
+      </c>
+      <c r="S73">
+        <v>850</v>
+      </c>
+      <c r="T73">
+        <v>0.5</v>
+      </c>
+      <c r="U73" t="s">
+        <v>42</v>
+      </c>
+      <c r="X73" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>11377</v>
+      </c>
+      <c r="C74">
+        <v>11377</v>
+      </c>
+      <c r="D74">
+        <v>11377</v>
+      </c>
+      <c r="E74" t="s">
+        <v>87</v>
+      </c>
+      <c r="F74" t="s">
+        <v>17</v>
+      </c>
+      <c r="G74" t="s">
+        <v>18</v>
+      </c>
+      <c r="H74" t="s">
+        <v>38</v>
+      </c>
+      <c r="I74" t="s">
+        <v>20</v>
+      </c>
+      <c r="J74" t="s">
+        <v>97</v>
+      </c>
+      <c r="K74" t="s">
+        <v>19</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="M74">
+        <v>30</v>
+      </c>
+      <c r="N74" t="s">
+        <v>32</v>
+      </c>
+      <c r="O74" t="s">
+        <v>19</v>
+      </c>
+      <c r="P74" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q74">
+        <v>3373</v>
+      </c>
+      <c r="R74" t="s">
+        <v>106</v>
+      </c>
+      <c r="S74" s="2">
+        <v>650</v>
+      </c>
+      <c r="T74">
+        <v>0.5</v>
+      </c>
+      <c r="U74" t="s">
+        <v>42</v>
+      </c>
+      <c r="X74" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>11377</v>
+      </c>
+      <c r="C75">
+        <v>11377</v>
+      </c>
+      <c r="D75">
+        <v>11377</v>
+      </c>
+      <c r="E75" t="s">
+        <v>87</v>
+      </c>
+      <c r="F75" t="s">
+        <v>17</v>
+      </c>
+      <c r="G75" t="s">
+        <v>18</v>
+      </c>
+      <c r="H75" t="s">
+        <v>38</v>
+      </c>
+      <c r="I75" t="s">
+        <v>20</v>
+      </c>
+      <c r="J75" t="s">
+        <v>98</v>
+      </c>
+      <c r="K75" t="s">
+        <v>19</v>
+      </c>
+      <c r="L75">
+        <v>2</v>
+      </c>
+      <c r="M75">
+        <v>65</v>
+      </c>
+      <c r="N75" t="s">
+        <v>32</v>
+      </c>
+      <c r="O75" t="s">
+        <v>19</v>
+      </c>
+      <c r="P75" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q75">
+        <v>1993</v>
+      </c>
+      <c r="R75" t="s">
+        <v>107</v>
+      </c>
+      <c r="S75">
+        <v>351</v>
+      </c>
+      <c r="T75">
+        <v>0.5</v>
+      </c>
+      <c r="U75" t="s">
+        <v>42</v>
+      </c>
+      <c r="X75" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>11377</v>
+      </c>
+      <c r="C76">
+        <v>11377</v>
+      </c>
+      <c r="D76">
+        <v>11377</v>
+      </c>
+      <c r="E76" t="s">
+        <v>87</v>
+      </c>
+      <c r="F76" t="s">
+        <v>17</v>
+      </c>
+      <c r="G76" t="s">
+        <v>18</v>
+      </c>
+      <c r="H76" t="s">
+        <v>38</v>
+      </c>
+      <c r="I76" t="s">
+        <v>20</v>
+      </c>
+      <c r="J76" t="s">
+        <v>99</v>
+      </c>
+      <c r="K76" t="s">
+        <v>19</v>
+      </c>
+      <c r="L76">
+        <v>3</v>
+      </c>
+      <c r="M76">
+        <v>99</v>
+      </c>
+      <c r="N76" t="s">
+        <v>32</v>
+      </c>
+      <c r="O76" t="s">
+        <v>19</v>
+      </c>
+      <c r="P76" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q76">
+        <v>1324</v>
+      </c>
+      <c r="R76" t="s">
+        <v>108</v>
+      </c>
+      <c r="S76" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T76">
+        <v>0.5</v>
+      </c>
+      <c r="U76" t="s">
+        <v>42</v>
+      </c>
+      <c r="X76" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>11377</v>
+      </c>
+      <c r="C77">
+        <v>11377</v>
+      </c>
+      <c r="D77">
+        <v>11377</v>
+      </c>
+      <c r="E77" t="s">
+        <v>87</v>
+      </c>
+      <c r="F77" t="s">
+        <v>17</v>
+      </c>
+      <c r="G77" t="s">
+        <v>18</v>
+      </c>
+      <c r="H77" t="s">
+        <v>38</v>
+      </c>
+      <c r="I77" t="s">
+        <v>20</v>
+      </c>
+      <c r="J77" t="s">
+        <v>100</v>
+      </c>
+      <c r="K77" t="s">
+        <v>19</v>
+      </c>
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="M77">
+        <v>30</v>
+      </c>
+      <c r="N77" t="s">
+        <v>32</v>
+      </c>
+      <c r="O77" t="s">
+        <v>19</v>
+      </c>
+      <c r="P77" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q77">
+        <v>3481</v>
+      </c>
+      <c r="R77" t="s">
+        <v>110</v>
+      </c>
+      <c r="S77" s="2">
+        <v>967</v>
+      </c>
+      <c r="T77">
+        <v>0.5</v>
+      </c>
+      <c r="U77" t="s">
+        <v>42</v>
+      </c>
+      <c r="X77" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y77" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>11377</v>
+      </c>
+      <c r="C78">
+        <v>11377</v>
+      </c>
+      <c r="D78">
+        <v>11377</v>
+      </c>
+      <c r="E78" t="s">
+        <v>87</v>
+      </c>
+      <c r="F78" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78" t="s">
+        <v>18</v>
+      </c>
+      <c r="H78" t="s">
+        <v>38</v>
+      </c>
+      <c r="I78" t="s">
+        <v>20</v>
+      </c>
+      <c r="J78" t="s">
+        <v>101</v>
+      </c>
+      <c r="K78" t="s">
+        <v>19</v>
+      </c>
+      <c r="L78">
+        <v>2</v>
+      </c>
+      <c r="M78">
+        <v>65</v>
+      </c>
+      <c r="N78" t="s">
+        <v>32</v>
+      </c>
+      <c r="O78" t="s">
+        <v>19</v>
+      </c>
+      <c r="P78" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q78">
+        <v>3287</v>
+      </c>
+      <c r="R78" t="s">
+        <v>111</v>
+      </c>
+      <c r="S78" s="2">
+        <v>652</v>
+      </c>
+      <c r="T78">
+        <v>0.5</v>
+      </c>
+      <c r="U78" t="s">
+        <v>42</v>
+      </c>
+      <c r="X78" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>11377</v>
+      </c>
+      <c r="C79">
+        <v>11377</v>
+      </c>
+      <c r="D79">
+        <v>11377</v>
+      </c>
+      <c r="E79" t="s">
+        <v>87</v>
+      </c>
+      <c r="F79" t="s">
+        <v>17</v>
+      </c>
+      <c r="G79" t="s">
+        <v>18</v>
+      </c>
+      <c r="H79" t="s">
+        <v>38</v>
+      </c>
+      <c r="I79" t="s">
+        <v>20</v>
+      </c>
+      <c r="J79" t="s">
+        <v>102</v>
+      </c>
+      <c r="K79" t="s">
+        <v>19</v>
+      </c>
+      <c r="L79">
+        <v>3</v>
+      </c>
+      <c r="M79">
+        <v>99</v>
+      </c>
+      <c r="N79" t="s">
+        <v>32</v>
+      </c>
+      <c r="O79" t="s">
+        <v>19</v>
+      </c>
+      <c r="P79" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q79">
+        <v>1369</v>
+      </c>
+      <c r="R79" t="s">
+        <v>112</v>
+      </c>
+      <c r="S79" s="2">
+        <v>467</v>
+      </c>
+      <c r="T79">
+        <v>0.5</v>
+      </c>
+      <c r="U79" t="s">
+        <v>42</v>
+      </c>
+      <c r="X79" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>11377</v>
+      </c>
+      <c r="C80">
+        <v>11377</v>
+      </c>
+      <c r="D80">
+        <v>11377</v>
+      </c>
+      <c r="E80" t="s">
+        <v>93</v>
+      </c>
+      <c r="F80" t="s">
+        <v>17</v>
+      </c>
+      <c r="G80" t="s">
+        <v>25</v>
+      </c>
+      <c r="H80" t="s">
+        <v>19</v>
+      </c>
+      <c r="I80" t="s">
+        <v>20</v>
+      </c>
+      <c r="J80" t="s">
+        <v>19</v>
+      </c>
+      <c r="K80" t="s">
+        <v>19</v>
+      </c>
+      <c r="L80">
+        <v>13</v>
+      </c>
+      <c r="M80">
+        <v>775</v>
+      </c>
+      <c r="N80" t="s">
+        <v>21</v>
+      </c>
+      <c r="O80" t="s">
+        <v>22</v>
+      </c>
+      <c r="P80" t="s">
+        <v>23</v>
+      </c>
+      <c r="X80" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>11377</v>
+      </c>
+      <c r="C81">
+        <v>11377</v>
+      </c>
+      <c r="D81">
+        <v>11377</v>
+      </c>
+      <c r="E81" t="s">
+        <v>87</v>
+      </c>
+      <c r="F81" t="s">
+        <v>17</v>
+      </c>
+      <c r="G81" t="s">
+        <v>18</v>
+      </c>
+      <c r="H81" t="s">
+        <v>19</v>
+      </c>
+      <c r="I81" t="s">
+        <v>20</v>
+      </c>
+      <c r="J81" t="s">
+        <v>19</v>
+      </c>
+      <c r="K81" t="s">
+        <v>19</v>
+      </c>
+      <c r="L81">
+        <v>8</v>
+      </c>
+      <c r="M81">
+        <v>360</v>
+      </c>
+      <c r="N81" t="s">
+        <v>21</v>
+      </c>
+      <c r="O81" t="s">
+        <v>22</v>
+      </c>
+      <c r="P81" t="s">
+        <v>23</v>
+      </c>
+      <c r="X81" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>11377</v>
+      </c>
+      <c r="C82">
+        <v>11377</v>
+      </c>
+      <c r="D82">
+        <v>11377</v>
+      </c>
+      <c r="E82" t="s">
+        <v>87</v>
+      </c>
+      <c r="F82" t="s">
+        <v>17</v>
+      </c>
+      <c r="G82" t="s">
+        <v>33</v>
+      </c>
+      <c r="H82" t="s">
+        <v>19</v>
+      </c>
+      <c r="I82" t="s">
+        <v>20</v>
+      </c>
+      <c r="J82" t="s">
+        <v>19</v>
+      </c>
+      <c r="K82" t="s">
+        <v>19</v>
+      </c>
+      <c r="L82">
+        <v>2</v>
+      </c>
+      <c r="M82">
+        <v>55</v>
+      </c>
+      <c r="N82" t="s">
+        <v>21</v>
+      </c>
+      <c r="O82" t="s">
+        <v>22</v>
+      </c>
+      <c r="P82" t="s">
+        <v>23</v>
+      </c>
+      <c r="X82" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="X83" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
For 100 test data
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-sdutta2\ATaC_iCargo_WorkingDirectory\icargoUiAutomate_7thJan\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2024\Excel_6thJan\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0D79C4-CB8B-44B8-8484-2FC69E31D0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2657E18-5F8B-4950-85F4-F0AB81D7D864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{16092AE6-4963-404B-A94C-F9A0B99B87F0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{16092AE6-4963-404B-A94C-F9A0B99B87F0}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LTE001_ACC_00001!$A$1:$Y$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LTE001_ACC_00001!$A$1:$Y$88</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="114">
   <si>
     <t>AgentCode</t>
   </si>
@@ -762,10 +762,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13A9B56-5E6E-4A35-9DD7-E48E0C4AA254}">
-  <dimension ref="A1:Y85"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:Y88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -876,7 +877,7 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>35</v>
@@ -929,7 +930,7 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -982,7 +983,7 @@
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
         <v>41</v>
@@ -1138,13 +1139,13 @@
         <v>11377</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
         <v>28</v>
@@ -1159,10 +1160,10 @@
         <v>28</v>
       </c>
       <c r="L7">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>750</v>
+        <v>100</v>
       </c>
       <c r="N7" t="s">
         <v>30</v>
@@ -1181,23 +1182,23 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
+      <c r="A8">
+        <v>11377</v>
+      </c>
+      <c r="C8">
+        <v>11377</v>
       </c>
       <c r="D8">
-        <v>10763</v>
+        <v>11377</v>
       </c>
       <c r="E8" t="s">
         <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
         <v>28</v>
@@ -1212,16 +1213,16 @@
         <v>28</v>
       </c>
       <c r="L8">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="M8">
-        <v>775</v>
+        <v>600</v>
       </c>
       <c r="N8" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P8" t="s">
         <v>32</v>
@@ -1230,33 +1231,33 @@
         <v>33</v>
       </c>
       <c r="Y8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
+      <c r="A9">
+        <v>11377</v>
+      </c>
+      <c r="C9">
+        <v>11377</v>
       </c>
       <c r="D9">
-        <v>10763</v>
+        <v>11377</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="H9" t="s">
         <v>28</v>
       </c>
-      <c r="I9">
-        <v>2199</v>
+      <c r="I9" t="s">
+        <v>29</v>
       </c>
       <c r="J9" t="s">
         <v>28</v>
@@ -1265,16 +1266,16 @@
         <v>28</v>
       </c>
       <c r="L9">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="M9">
-        <v>360</v>
+        <v>750</v>
       </c>
       <c r="N9" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P9" t="s">
         <v>32</v>
@@ -1283,24 +1284,24 @@
         <v>33</v>
       </c>
       <c r="Y9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
+      <c r="A10">
+        <v>11377</v>
+      </c>
+      <c r="C10">
+        <v>11377</v>
       </c>
       <c r="D10">
-        <v>10763</v>
+        <v>11377</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
         <v>41</v>
@@ -1318,16 +1319,16 @@
         <v>28</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="M10">
-        <v>59</v>
+        <v>750</v>
       </c>
       <c r="N10" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P10" t="s">
         <v>32</v>
@@ -1336,7 +1337,7 @@
         <v>33</v>
       </c>
       <c r="Y10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.35">
@@ -1350,13 +1351,13 @@
         <v>10763</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
         <v>28</v>
@@ -1403,19 +1404,19 @@
         <v>10763</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H12" t="s">
         <v>28</v>
       </c>
-      <c r="I12" t="s">
-        <v>29</v>
+      <c r="I12">
+        <v>2199</v>
       </c>
       <c r="J12" t="s">
         <v>28</v>
@@ -1424,10 +1425,10 @@
         <v>28</v>
       </c>
       <c r="L12">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M12">
-        <v>59</v>
+        <v>360</v>
       </c>
       <c r="N12" t="s">
         <v>39</v>
@@ -1456,13 +1457,13 @@
         <v>10763</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="H13" t="s">
         <v>28</v>
@@ -1477,10 +1478,10 @@
         <v>28</v>
       </c>
       <c r="L13">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="M13">
-        <v>775</v>
+        <v>59</v>
       </c>
       <c r="N13" t="s">
         <v>39</v>
@@ -1499,100 +1500,85 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>11377</v>
-      </c>
-      <c r="C14">
-        <v>11377</v>
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
       </c>
       <c r="D14">
-        <v>11377</v>
+        <v>10763</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="H14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="I14" t="s">
         <v>29</v>
       </c>
       <c r="J14" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="K14" t="s">
         <v>28</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="M14">
-        <v>30</v>
+        <v>775</v>
       </c>
       <c r="N14" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P14" t="s">
         <v>32</v>
       </c>
-      <c r="Q14">
-        <v>8000</v>
-      </c>
-      <c r="R14" t="s">
-        <v>45</v>
-      </c>
-      <c r="S14" t="s">
-        <v>46</v>
-      </c>
-      <c r="T14">
-        <v>0.5</v>
-      </c>
-      <c r="U14" t="s">
-        <v>47</v>
-      </c>
       <c r="X14" t="s">
         <v>33</v>
       </c>
       <c r="Y14" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>11377</v>
-      </c>
-      <c r="C15">
-        <v>11377</v>
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
       </c>
       <c r="D15">
-        <v>11377</v>
+        <v>10763</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="I15" t="s">
         <v>29</v>
       </c>
       <c r="J15" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="K15" t="s">
         <v>28</v>
@@ -1601,105 +1587,75 @@
         <v>2</v>
       </c>
       <c r="M15">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="N15" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P15" t="s">
         <v>32</v>
       </c>
-      <c r="Q15">
-        <v>1845</v>
-      </c>
-      <c r="R15" t="s">
-        <v>51</v>
-      </c>
-      <c r="S15">
-        <v>954</v>
-      </c>
-      <c r="T15">
-        <v>0.5</v>
-      </c>
-      <c r="U15" t="s">
-        <v>47</v>
-      </c>
       <c r="X15" t="s">
         <v>33</v>
       </c>
       <c r="Y15" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>11377</v>
-      </c>
-      <c r="C16">
-        <v>11377</v>
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
       </c>
       <c r="D16">
-        <v>11377</v>
+        <v>10763</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="G16" t="s">
         <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="I16" t="s">
         <v>29</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="K16" t="s">
         <v>28</v>
       </c>
       <c r="L16">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="M16">
-        <v>99</v>
+        <v>775</v>
       </c>
       <c r="N16" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P16" t="s">
         <v>32</v>
       </c>
-      <c r="Q16">
-        <v>3110</v>
-      </c>
-      <c r="R16" t="s">
-        <v>54</v>
-      </c>
-      <c r="S16">
-        <v>570</v>
-      </c>
-      <c r="T16">
-        <v>0.5</v>
-      </c>
-      <c r="U16" t="s">
-        <v>47</v>
-      </c>
       <c r="X16" t="s">
         <v>33</v>
       </c>
       <c r="Y16" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.35">
@@ -1728,7 +1684,7 @@
         <v>29</v>
       </c>
       <c r="J17" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="K17" t="s">
         <v>28</v>
@@ -1740,22 +1696,22 @@
         <v>30</v>
       </c>
       <c r="N17" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O17" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P17" t="s">
         <v>32</v>
       </c>
       <c r="Q17">
-        <v>2807</v>
+        <v>8000</v>
       </c>
       <c r="R17" t="s">
-        <v>95</v>
-      </c>
-      <c r="S17" s="2">
-        <v>953</v>
+        <v>45</v>
+      </c>
+      <c r="S17" t="s">
+        <v>46</v>
       </c>
       <c r="T17">
         <v>0.5</v>
@@ -1781,10 +1737,10 @@
         <v>11377</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="G18" t="s">
         <v>27</v>
@@ -1796,7 +1752,7 @@
         <v>29</v>
       </c>
       <c r="J18" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="K18" t="s">
         <v>28</v>
@@ -1808,22 +1764,22 @@
         <v>65</v>
       </c>
       <c r="N18" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O18" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P18" t="s">
         <v>32</v>
       </c>
       <c r="Q18">
-        <v>1977</v>
+        <v>1845</v>
       </c>
       <c r="R18" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="S18">
-        <v>202</v>
+        <v>954</v>
       </c>
       <c r="T18">
         <v>0.5</v>
@@ -1849,10 +1805,10 @@
         <v>11377</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="G19" t="s">
         <v>27</v>
@@ -1864,7 +1820,7 @@
         <v>29</v>
       </c>
       <c r="J19" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="K19" t="s">
         <v>28</v>
@@ -1876,22 +1832,22 @@
         <v>99</v>
       </c>
       <c r="N19" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P19" t="s">
         <v>32</v>
       </c>
       <c r="Q19">
-        <v>1760</v>
+        <v>3110</v>
       </c>
       <c r="R19" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="S19">
-        <v>850</v>
+        <v>570</v>
       </c>
       <c r="T19">
         <v>0.5</v>
@@ -1917,7 +1873,7 @@
         <v>11377</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F20" t="s">
         <v>38</v>
@@ -1932,7 +1888,7 @@
         <v>29</v>
       </c>
       <c r="J20" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="K20" t="s">
         <v>28</v>
@@ -1953,13 +1909,13 @@
         <v>32</v>
       </c>
       <c r="Q20">
-        <v>3373</v>
+        <v>2807</v>
       </c>
       <c r="R20" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="S20" s="2">
-        <v>650</v>
+        <v>953</v>
       </c>
       <c r="T20">
         <v>0.5</v>
@@ -2000,7 +1956,7 @@
         <v>29</v>
       </c>
       <c r="J21" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="K21" t="s">
         <v>28</v>
@@ -2021,13 +1977,13 @@
         <v>32</v>
       </c>
       <c r="Q21">
-        <v>1993</v>
+        <v>1977</v>
       </c>
       <c r="R21" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="S21">
-        <v>351</v>
+        <v>202</v>
       </c>
       <c r="T21">
         <v>0.5</v>
@@ -2068,7 +2024,7 @@
         <v>29</v>
       </c>
       <c r="J22" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="K22" t="s">
         <v>28</v>
@@ -2089,13 +2045,13 @@
         <v>32</v>
       </c>
       <c r="Q22">
-        <v>1324</v>
+        <v>1760</v>
       </c>
       <c r="R22" t="s">
-        <v>105</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="S22">
+        <v>850</v>
       </c>
       <c r="T22">
         <v>0.5</v>
@@ -2121,7 +2077,7 @@
         <v>11377</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
         <v>38</v>
@@ -2136,7 +2092,7 @@
         <v>29</v>
       </c>
       <c r="J23" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="K23" t="s">
         <v>28</v>
@@ -2157,13 +2113,13 @@
         <v>32</v>
       </c>
       <c r="Q23">
-        <v>3481</v>
+        <v>3373</v>
       </c>
       <c r="R23" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="S23" s="2">
-        <v>967</v>
+        <v>650</v>
       </c>
       <c r="T23">
         <v>0.5</v>
@@ -2189,10 +2145,10 @@
         <v>11377</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="F24" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G24" t="s">
         <v>27</v>
@@ -2204,7 +2160,7 @@
         <v>29</v>
       </c>
       <c r="J24" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K24" t="s">
         <v>28</v>
@@ -2225,13 +2181,13 @@
         <v>32</v>
       </c>
       <c r="Q24">
-        <v>3287</v>
+        <v>1993</v>
       </c>
       <c r="R24" t="s">
-        <v>110</v>
-      </c>
-      <c r="S24" s="2">
-        <v>652</v>
+        <v>103</v>
+      </c>
+      <c r="S24">
+        <v>351</v>
       </c>
       <c r="T24">
         <v>0.5</v>
@@ -2257,10 +2213,10 @@
         <v>11377</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="F25" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="G25" t="s">
         <v>27</v>
@@ -2272,7 +2228,7 @@
         <v>29</v>
       </c>
       <c r="J25" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="K25" t="s">
         <v>28</v>
@@ -2293,13 +2249,13 @@
         <v>32</v>
       </c>
       <c r="Q25">
-        <v>1369</v>
+        <v>1324</v>
       </c>
       <c r="R25" t="s">
-        <v>112</v>
-      </c>
-      <c r="S25" s="2">
-        <v>467</v>
+        <v>105</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="T25">
         <v>0.5</v>
@@ -2325,10 +2281,10 @@
         <v>11377</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G26" t="s">
         <v>27</v>
@@ -2340,7 +2296,7 @@
         <v>29</v>
       </c>
       <c r="J26" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="K26" t="s">
         <v>28</v>
@@ -2352,22 +2308,22 @@
         <v>30</v>
       </c>
       <c r="N26" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P26" t="s">
         <v>32</v>
       </c>
       <c r="Q26">
-        <v>8000</v>
+        <v>3481</v>
       </c>
       <c r="R26" t="s">
-        <v>45</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>46</v>
+        <v>108</v>
+      </c>
+      <c r="S26" s="2">
+        <v>967</v>
       </c>
       <c r="T26">
         <v>0.5</v>
@@ -2393,10 +2349,10 @@
         <v>11377</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="G27" t="s">
         <v>27</v>
@@ -2408,7 +2364,7 @@
         <v>29</v>
       </c>
       <c r="J27" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="K27" t="s">
         <v>28</v>
@@ -2420,22 +2376,22 @@
         <v>65</v>
       </c>
       <c r="N27" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P27" t="s">
         <v>32</v>
       </c>
       <c r="Q27">
-        <v>1845</v>
+        <v>3287</v>
       </c>
       <c r="R27" t="s">
-        <v>51</v>
-      </c>
-      <c r="S27">
-        <v>954</v>
+        <v>110</v>
+      </c>
+      <c r="S27" s="2">
+        <v>652</v>
       </c>
       <c r="T27">
         <v>0.5</v>
@@ -2461,10 +2417,10 @@
         <v>11377</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="G28" t="s">
         <v>27</v>
@@ -2476,7 +2432,7 @@
         <v>29</v>
       </c>
       <c r="J28" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="K28" t="s">
         <v>28</v>
@@ -2488,22 +2444,22 @@
         <v>99</v>
       </c>
       <c r="N28" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P28" t="s">
         <v>32</v>
       </c>
       <c r="Q28">
-        <v>3110</v>
+        <v>1369</v>
       </c>
       <c r="R28" t="s">
-        <v>54</v>
-      </c>
-      <c r="S28">
-        <v>570</v>
+        <v>112</v>
+      </c>
+      <c r="S28" s="2">
+        <v>467</v>
       </c>
       <c r="T28">
         <v>0.5</v>
@@ -2544,7 +2500,7 @@
         <v>29</v>
       </c>
       <c r="J29" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="K29" t="s">
         <v>28</v>
@@ -2556,22 +2512,22 @@
         <v>30</v>
       </c>
       <c r="N29" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O29" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P29" t="s">
         <v>32</v>
       </c>
       <c r="Q29">
-        <v>2807</v>
+        <v>8000</v>
       </c>
       <c r="R29" t="s">
-        <v>95</v>
-      </c>
-      <c r="S29" s="2">
-        <v>953</v>
+        <v>45</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="T29">
         <v>0.5</v>
@@ -2612,7 +2568,7 @@
         <v>29</v>
       </c>
       <c r="J30" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="K30" t="s">
         <v>28</v>
@@ -2624,22 +2580,22 @@
         <v>65</v>
       </c>
       <c r="N30" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P30" t="s">
         <v>32</v>
       </c>
       <c r="Q30">
-        <v>1977</v>
+        <v>1845</v>
       </c>
       <c r="R30" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="S30">
-        <v>202</v>
+        <v>954</v>
       </c>
       <c r="T30">
         <v>0.5</v>
@@ -2680,7 +2636,7 @@
         <v>29</v>
       </c>
       <c r="J31" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="K31" t="s">
         <v>28</v>
@@ -2692,22 +2648,22 @@
         <v>99</v>
       </c>
       <c r="N31" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O31" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P31" t="s">
         <v>32</v>
       </c>
       <c r="Q31">
-        <v>1760</v>
+        <v>3110</v>
       </c>
       <c r="R31" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="S31">
-        <v>850</v>
+        <v>570</v>
       </c>
       <c r="T31">
         <v>0.5</v>
@@ -2733,7 +2689,7 @@
         <v>11377</v>
       </c>
       <c r="E32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F32" t="s">
         <v>26</v>
@@ -2748,7 +2704,7 @@
         <v>29</v>
       </c>
       <c r="J32" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="K32" t="s">
         <v>28</v>
@@ -2769,13 +2725,13 @@
         <v>32</v>
       </c>
       <c r="Q32">
-        <v>3373</v>
+        <v>2807</v>
       </c>
       <c r="R32" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="S32" s="2">
-        <v>650</v>
+        <v>953</v>
       </c>
       <c r="T32">
         <v>0.5</v>
@@ -2801,7 +2757,7 @@
         <v>11377</v>
       </c>
       <c r="E33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F33" t="s">
         <v>26</v>
@@ -2816,7 +2772,7 @@
         <v>29</v>
       </c>
       <c r="J33" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="K33" t="s">
         <v>28</v>
@@ -2837,13 +2793,13 @@
         <v>32</v>
       </c>
       <c r="Q33">
-        <v>1993</v>
+        <v>1977</v>
       </c>
       <c r="R33" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="S33">
-        <v>351</v>
+        <v>202</v>
       </c>
       <c r="T33">
         <v>0.5</v>
@@ -2869,7 +2825,7 @@
         <v>11377</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F34" t="s">
         <v>26</v>
@@ -2884,7 +2840,7 @@
         <v>29</v>
       </c>
       <c r="J34" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="K34" t="s">
         <v>28</v>
@@ -2905,13 +2861,13 @@
         <v>32</v>
       </c>
       <c r="Q34">
-        <v>1324</v>
+        <v>1760</v>
       </c>
       <c r="R34" t="s">
-        <v>105</v>
-      </c>
-      <c r="S34" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="S34">
+        <v>850</v>
       </c>
       <c r="T34">
         <v>0.5</v>
@@ -2952,7 +2908,7 @@
         <v>29</v>
       </c>
       <c r="J35" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="K35" t="s">
         <v>28</v>
@@ -2973,13 +2929,13 @@
         <v>32</v>
       </c>
       <c r="Q35">
-        <v>3481</v>
+        <v>3373</v>
       </c>
       <c r="R35" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="S35" s="2">
-        <v>967</v>
+        <v>650</v>
       </c>
       <c r="T35">
         <v>0.5</v>
@@ -3020,7 +2976,7 @@
         <v>29</v>
       </c>
       <c r="J36" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K36" t="s">
         <v>28</v>
@@ -3041,13 +2997,13 @@
         <v>32</v>
       </c>
       <c r="Q36">
-        <v>3287</v>
+        <v>1993</v>
       </c>
       <c r="R36" t="s">
-        <v>110</v>
-      </c>
-      <c r="S36" s="2">
-        <v>652</v>
+        <v>103</v>
+      </c>
+      <c r="S36">
+        <v>351</v>
       </c>
       <c r="T36">
         <v>0.5</v>
@@ -3088,7 +3044,7 @@
         <v>29</v>
       </c>
       <c r="J37" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="K37" t="s">
         <v>28</v>
@@ -3109,13 +3065,13 @@
         <v>32</v>
       </c>
       <c r="Q37">
-        <v>1369</v>
+        <v>1324</v>
       </c>
       <c r="R37" t="s">
-        <v>112</v>
-      </c>
-      <c r="S37" s="2">
-        <v>467</v>
+        <v>105</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="T37">
         <v>0.5</v>
@@ -3141,46 +3097,61 @@
         <v>11377</v>
       </c>
       <c r="E38" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F38" t="s">
         <v>26</v>
       </c>
       <c r="G38" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H38" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="I38" t="s">
         <v>29</v>
       </c>
       <c r="J38" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="K38" t="s">
         <v>28</v>
       </c>
       <c r="L38">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="M38">
-        <v>775</v>
+        <v>30</v>
       </c>
       <c r="N38" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O38" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P38" t="s">
         <v>32</v>
       </c>
+      <c r="Q38">
+        <v>3481</v>
+      </c>
+      <c r="R38" t="s">
+        <v>108</v>
+      </c>
+      <c r="S38" s="2">
+        <v>967</v>
+      </c>
+      <c r="T38">
+        <v>0.5</v>
+      </c>
+      <c r="U38" t="s">
+        <v>47</v>
+      </c>
       <c r="X38" t="s">
         <v>33</v>
       </c>
       <c r="Y38" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.35">
@@ -3203,37 +3174,52 @@
         <v>27</v>
       </c>
       <c r="H39" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="I39" t="s">
         <v>29</v>
       </c>
       <c r="J39" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="K39" t="s">
         <v>28</v>
       </c>
       <c r="L39">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M39">
-        <v>360</v>
+        <v>65</v>
       </c>
       <c r="N39" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O39" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P39" t="s">
         <v>32</v>
       </c>
+      <c r="Q39">
+        <v>3287</v>
+      </c>
+      <c r="R39" t="s">
+        <v>110</v>
+      </c>
+      <c r="S39" s="2">
+        <v>652</v>
+      </c>
+      <c r="T39">
+        <v>0.5</v>
+      </c>
+      <c r="U39" t="s">
+        <v>47</v>
+      </c>
       <c r="X39" t="s">
         <v>33</v>
       </c>
       <c r="Y39" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">
@@ -3253,40 +3239,55 @@
         <v>26</v>
       </c>
       <c r="G40" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="H40" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="I40" t="s">
         <v>29</v>
       </c>
       <c r="J40" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="K40" t="s">
         <v>28</v>
       </c>
       <c r="L40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M40">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="N40" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O40" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P40" t="s">
         <v>32</v>
       </c>
+      <c r="Q40">
+        <v>1369</v>
+      </c>
+      <c r="R40" t="s">
+        <v>112</v>
+      </c>
+      <c r="S40" s="2">
+        <v>467</v>
+      </c>
+      <c r="T40">
+        <v>0.5</v>
+      </c>
+      <c r="U40" t="s">
+        <v>47</v>
+      </c>
       <c r="X40" t="s">
         <v>33</v>
       </c>
       <c r="Y40" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.35">
@@ -3300,19 +3301,19 @@
         <v>11377</v>
       </c>
       <c r="E41" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F41" t="s">
         <v>26</v>
       </c>
       <c r="G41" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H41" t="s">
         <v>28</v>
       </c>
-      <c r="I41" s="1" t="s">
-        <v>55</v>
+      <c r="I41" t="s">
+        <v>29</v>
       </c>
       <c r="J41" t="s">
         <v>28</v>
@@ -3353,10 +3354,10 @@
         <v>11377</v>
       </c>
       <c r="E42" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="F42" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="G42" t="s">
         <v>27</v>
@@ -3364,8 +3365,8 @@
       <c r="H42" t="s">
         <v>28</v>
       </c>
-      <c r="I42">
-        <v>2199</v>
+      <c r="I42" t="s">
+        <v>29</v>
       </c>
       <c r="J42" t="s">
         <v>28</v>
@@ -3406,19 +3407,19 @@
         <v>11377</v>
       </c>
       <c r="E43" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F43" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G43" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="H43" t="s">
         <v>28</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>58</v>
+      <c r="I43" t="s">
+        <v>29</v>
       </c>
       <c r="J43" t="s">
         <v>28</v>
@@ -3459,19 +3460,19 @@
         <v>11377</v>
       </c>
       <c r="E44" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F44" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G44" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H44" t="s">
         <v>28</v>
       </c>
-      <c r="I44" t="s">
-        <v>29</v>
+      <c r="I44" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="J44" t="s">
         <v>28</v>
@@ -3480,16 +3481,16 @@
         <v>28</v>
       </c>
       <c r="L44">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="M44">
-        <v>100</v>
+        <v>775</v>
       </c>
       <c r="N44" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O44" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P44" t="s">
         <v>32</v>
@@ -3498,7 +3499,7 @@
         <v>33</v>
       </c>
       <c r="Y44" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.35">
@@ -3515,7 +3516,7 @@
         <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G45" t="s">
         <v>27</v>
@@ -3523,8 +3524,8 @@
       <c r="H45" t="s">
         <v>28</v>
       </c>
-      <c r="I45" t="s">
-        <v>29</v>
+      <c r="I45">
+        <v>2199</v>
       </c>
       <c r="J45" t="s">
         <v>28</v>
@@ -3536,13 +3537,13 @@
         <v>8</v>
       </c>
       <c r="M45">
-        <v>600</v>
+        <v>360</v>
       </c>
       <c r="N45" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O45" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P45" t="s">
         <v>32</v>
@@ -3551,7 +3552,7 @@
         <v>33</v>
       </c>
       <c r="Y45" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.35">
@@ -3565,19 +3566,19 @@
         <v>11377</v>
       </c>
       <c r="E46" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="F46" t="s">
         <v>38</v>
       </c>
       <c r="G46" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="H46" t="s">
         <v>28</v>
       </c>
-      <c r="I46" t="s">
-        <v>29</v>
+      <c r="I46" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="J46" t="s">
         <v>28</v>
@@ -3586,16 +3587,16 @@
         <v>28</v>
       </c>
       <c r="L46">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="M46">
-        <v>750</v>
+        <v>55</v>
       </c>
       <c r="N46" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O46" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P46" t="s">
         <v>32</v>
@@ -3604,7 +3605,7 @@
         <v>33</v>
       </c>
       <c r="Y46" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.35">
@@ -3618,10 +3619,10 @@
         <v>11377</v>
       </c>
       <c r="E47" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F47" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="G47" t="s">
         <v>35</v>
@@ -3671,10 +3672,10 @@
         <v>11377</v>
       </c>
       <c r="E48" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F48" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="G48" t="s">
         <v>27</v>
@@ -3724,10 +3725,10 @@
         <v>11377</v>
       </c>
       <c r="E49" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="F49" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="G49" t="s">
         <v>41</v>
@@ -3777,10 +3778,10 @@
         <v>11377</v>
       </c>
       <c r="E50" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="F50" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G50" t="s">
         <v>35</v>
@@ -3798,10 +3799,10 @@
         <v>28</v>
       </c>
       <c r="L50">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="M50">
-        <v>750</v>
+        <v>100</v>
       </c>
       <c r="N50" t="s">
         <v>39</v>
@@ -3816,7 +3817,7 @@
         <v>33</v>
       </c>
       <c r="Y50" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.35">
@@ -3830,10 +3831,10 @@
         <v>11377</v>
       </c>
       <c r="E51" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="F51" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G51" t="s">
         <v>27</v>
@@ -3851,10 +3852,10 @@
         <v>28</v>
       </c>
       <c r="L51">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="M51">
-        <v>360</v>
+        <v>600</v>
       </c>
       <c r="N51" t="s">
         <v>39</v>
@@ -3869,7 +3870,7 @@
         <v>33</v>
       </c>
       <c r="Y51" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.35">
@@ -3883,10 +3884,10 @@
         <v>11377</v>
       </c>
       <c r="E52" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="F52" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G52" t="s">
         <v>41</v>
@@ -3904,10 +3905,10 @@
         <v>28</v>
       </c>
       <c r="L52">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="M52">
-        <v>55</v>
+        <v>750</v>
       </c>
       <c r="N52" t="s">
         <v>39</v>
@@ -3922,7 +3923,7 @@
         <v>33</v>
       </c>
       <c r="Y52" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.35">
@@ -3936,10 +3937,10 @@
         <v>11377</v>
       </c>
       <c r="E53" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F53" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G53" t="s">
         <v>35</v>
@@ -3989,10 +3990,10 @@
         <v>11377</v>
       </c>
       <c r="E54" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F54" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G54" t="s">
         <v>27</v>
@@ -4042,10 +4043,10 @@
         <v>11377</v>
       </c>
       <c r="E55" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G55" t="s">
         <v>41</v>
@@ -4095,10 +4096,10 @@
         <v>11377</v>
       </c>
       <c r="E56" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="F56" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="G56" t="s">
         <v>35</v>
@@ -4116,28 +4117,25 @@
         <v>28</v>
       </c>
       <c r="L56">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="M56">
-        <v>59</v>
+        <v>750</v>
       </c>
       <c r="N56" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P56" t="s">
         <v>32</v>
       </c>
-      <c r="V56">
-        <v>1</v>
-      </c>
       <c r="X56" t="s">
         <v>33</v>
       </c>
       <c r="Y56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.35">
@@ -4151,10 +4149,10 @@
         <v>11377</v>
       </c>
       <c r="E57" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="F57" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G57" t="s">
         <v>27</v>
@@ -4162,8 +4160,8 @@
       <c r="H57" t="s">
         <v>28</v>
       </c>
-      <c r="I57">
-        <v>2199</v>
+      <c r="I57" t="s">
+        <v>29</v>
       </c>
       <c r="J57" t="s">
         <v>28</v>
@@ -4172,28 +4170,25 @@
         <v>28</v>
       </c>
       <c r="L57">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M57">
-        <v>324</v>
+        <v>360</v>
       </c>
       <c r="N57" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O57" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P57" t="s">
         <v>32</v>
       </c>
-      <c r="V57">
-        <v>1</v>
-      </c>
       <c r="X57" t="s">
         <v>33</v>
       </c>
       <c r="Y57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.35">
@@ -4207,10 +4202,10 @@
         <v>11377</v>
       </c>
       <c r="E58" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="F58" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G58" t="s">
         <v>41</v>
@@ -4231,28 +4226,25 @@
         <v>2</v>
       </c>
       <c r="M58">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N58" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O58" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P58" t="s">
         <v>32</v>
       </c>
-      <c r="V58">
-        <v>1</v>
-      </c>
       <c r="X58" t="s">
         <v>33</v>
       </c>
       <c r="Y58" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>11377</v>
       </c>
@@ -4266,10 +4258,10 @@
         <v>26</v>
       </c>
       <c r="F59" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G59" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="H59" t="s">
         <v>28</v>
@@ -4308,7 +4300,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>11377</v>
       </c>
@@ -4322,16 +4314,16 @@
         <v>26</v>
       </c>
       <c r="F60" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G60" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H60" t="s">
         <v>28</v>
       </c>
-      <c r="I60" t="s">
-        <v>29</v>
+      <c r="I60">
+        <v>2199</v>
       </c>
       <c r="J60" t="s">
         <v>28</v>
@@ -4340,28 +4332,31 @@
         <v>28</v>
       </c>
       <c r="L60">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M60">
-        <v>775</v>
+        <v>324</v>
       </c>
       <c r="N60" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O60" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P60" t="s">
         <v>32</v>
       </c>
+      <c r="V60">
+        <v>1</v>
+      </c>
       <c r="X60" t="s">
         <v>33</v>
       </c>
       <c r="Y60" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>11377</v>
       </c>
@@ -4375,10 +4370,10 @@
         <v>26</v>
       </c>
       <c r="F61" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G61" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="H61" t="s">
         <v>28</v>
@@ -4393,28 +4388,31 @@
         <v>28</v>
       </c>
       <c r="L61">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M61">
-        <v>200</v>
+        <v>59</v>
       </c>
       <c r="N61" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O61" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P61" t="s">
         <v>32</v>
       </c>
+      <c r="V61">
+        <v>1</v>
+      </c>
       <c r="X61" t="s">
         <v>33</v>
       </c>
       <c r="Y61" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>11377</v>
       </c>
@@ -4431,7 +4429,7 @@
         <v>49</v>
       </c>
       <c r="G62" t="s">
-        <v>27</v>
+        <v>113</v>
       </c>
       <c r="H62" t="s">
         <v>28</v>
@@ -4446,28 +4444,31 @@
         <v>28</v>
       </c>
       <c r="L62">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M62">
-        <v>840</v>
+        <v>59</v>
       </c>
       <c r="N62" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O62" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P62" t="s">
         <v>32</v>
       </c>
+      <c r="V62">
+        <v>1</v>
+      </c>
       <c r="X62" t="s">
         <v>33</v>
       </c>
       <c r="Y62" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>11377</v>
       </c>
@@ -4481,7 +4482,7 @@
         <v>26</v>
       </c>
       <c r="F63" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G63" t="s">
         <v>35</v>
@@ -4499,31 +4500,28 @@
         <v>28</v>
       </c>
       <c r="L63">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="M63">
-        <v>59</v>
+        <v>775</v>
       </c>
       <c r="N63" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O63" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P63" t="s">
         <v>32</v>
       </c>
-      <c r="V63" t="s">
-        <v>65</v>
-      </c>
       <c r="X63" t="s">
         <v>33</v>
       </c>
       <c r="Y63" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>11377</v>
       </c>
@@ -4545,8 +4543,8 @@
       <c r="H64" t="s">
         <v>28</v>
       </c>
-      <c r="I64">
-        <v>2199</v>
+      <c r="I64" t="s">
+        <v>29</v>
       </c>
       <c r="J64" t="s">
         <v>28</v>
@@ -4555,107 +4553,104 @@
         <v>28</v>
       </c>
       <c r="L64">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="M64">
-        <v>259</v>
+        <v>200</v>
       </c>
       <c r="N64" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O64" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P64" t="s">
         <v>32</v>
       </c>
-      <c r="V64" t="s">
+      <c r="X64" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>11377</v>
+      </c>
+      <c r="C65">
+        <v>11377</v>
+      </c>
+      <c r="D65">
+        <v>11377</v>
+      </c>
+      <c r="E65" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" t="s">
+        <v>49</v>
+      </c>
+      <c r="G65" t="s">
+        <v>27</v>
+      </c>
+      <c r="H65" t="s">
+        <v>28</v>
+      </c>
+      <c r="I65" t="s">
+        <v>29</v>
+      </c>
+      <c r="J65" t="s">
+        <v>28</v>
+      </c>
+      <c r="K65" t="s">
+        <v>28</v>
+      </c>
+      <c r="L65">
+        <v>8</v>
+      </c>
+      <c r="M65">
+        <v>840</v>
+      </c>
+      <c r="N65" t="s">
+        <v>39</v>
+      </c>
+      <c r="O65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P65" t="s">
+        <v>32</v>
+      </c>
+      <c r="X65" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>11377</v>
+      </c>
+      <c r="C66">
+        <v>11377</v>
+      </c>
+      <c r="D66">
+        <v>11377</v>
+      </c>
+      <c r="E66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" t="s">
         <v>38</v>
       </c>
-      <c r="X64" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y64" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>11377</v>
-      </c>
-      <c r="C65">
-        <v>11377</v>
-      </c>
-      <c r="D65">
-        <v>11377</v>
-      </c>
-      <c r="E65" t="s">
-        <v>67</v>
-      </c>
-      <c r="F65" t="s">
-        <v>26</v>
-      </c>
-      <c r="G65" t="s">
+      <c r="G66" t="s">
         <v>35</v>
       </c>
-      <c r="H65" t="s">
-        <v>28</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J65" t="s">
-        <v>28</v>
-      </c>
-      <c r="K65" t="s">
-        <v>28</v>
-      </c>
-      <c r="L65">
-        <v>13</v>
-      </c>
-      <c r="M65">
-        <v>775</v>
-      </c>
-      <c r="N65" t="s">
-        <v>30</v>
-      </c>
-      <c r="O65" t="s">
-        <v>31</v>
-      </c>
-      <c r="P65" t="s">
-        <v>32</v>
-      </c>
-      <c r="X65" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y65" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>11377</v>
-      </c>
-      <c r="C66">
-        <v>11377</v>
-      </c>
-      <c r="D66">
-        <v>11377</v>
-      </c>
-      <c r="E66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F66" t="s">
-        <v>26</v>
-      </c>
-      <c r="G66" t="s">
-        <v>27</v>
-      </c>
       <c r="H66" t="s">
         <v>28</v>
       </c>
-      <c r="I66">
-        <v>2199</v>
+      <c r="I66" t="s">
+        <v>29</v>
       </c>
       <c r="J66" t="s">
         <v>28</v>
@@ -4664,10 +4659,10 @@
         <v>28</v>
       </c>
       <c r="L66">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M66">
-        <v>360</v>
+        <v>59</v>
       </c>
       <c r="N66" t="s">
         <v>30</v>
@@ -4678,14 +4673,17 @@
       <c r="P66" t="s">
         <v>32</v>
       </c>
+      <c r="V66" t="s">
+        <v>65</v>
+      </c>
       <c r="X66" t="s">
         <v>33</v>
       </c>
       <c r="Y66" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>11377</v>
       </c>
@@ -4696,19 +4694,19 @@
         <v>11377</v>
       </c>
       <c r="E67" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="F67" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="G67" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="H67" t="s">
         <v>28</v>
       </c>
-      <c r="I67" t="s">
-        <v>29</v>
+      <c r="I67">
+        <v>2199</v>
       </c>
       <c r="J67" t="s">
         <v>28</v>
@@ -4717,10 +4715,10 @@
         <v>28</v>
       </c>
       <c r="L67">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="M67">
-        <v>59</v>
+        <v>259</v>
       </c>
       <c r="N67" t="s">
         <v>30</v>
@@ -4731,28 +4729,31 @@
       <c r="P67" t="s">
         <v>32</v>
       </c>
+      <c r="V67" t="s">
+        <v>38</v>
+      </c>
       <c r="X67" t="s">
         <v>33</v>
       </c>
       <c r="Y67" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>36</v>
-      </c>
-      <c r="B68" t="s">
-        <v>37</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>11377</v>
+      </c>
+      <c r="C68">
+        <v>11377</v>
       </c>
       <c r="D68">
-        <v>10763</v>
+        <v>11377</v>
       </c>
       <c r="E68" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F68" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G68" t="s">
         <v>35</v>
@@ -4760,8 +4761,8 @@
       <c r="H68" t="s">
         <v>28</v>
       </c>
-      <c r="I68" t="s">
-        <v>29</v>
+      <c r="I68" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="J68" t="s">
         <v>28</v>
@@ -4776,10 +4777,10 @@
         <v>775</v>
       </c>
       <c r="N68" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O68" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P68" t="s">
         <v>32</v>
@@ -4788,24 +4789,24 @@
         <v>33</v>
       </c>
       <c r="Y68" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>36</v>
-      </c>
-      <c r="B69" t="s">
-        <v>37</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>11377</v>
+      </c>
+      <c r="C69">
+        <v>11377</v>
       </c>
       <c r="D69">
-        <v>10763</v>
+        <v>11377</v>
       </c>
       <c r="E69" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F69" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G69" t="s">
         <v>27</v>
@@ -4829,10 +4830,10 @@
         <v>360</v>
       </c>
       <c r="N69" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O69" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P69" t="s">
         <v>32</v>
@@ -4841,24 +4842,24 @@
         <v>33</v>
       </c>
       <c r="Y69" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>36</v>
-      </c>
-      <c r="B70" t="s">
-        <v>37</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>11377</v>
+      </c>
+      <c r="C70">
+        <v>11377</v>
       </c>
       <c r="D70">
-        <v>10763</v>
+        <v>11377</v>
       </c>
       <c r="E70" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F70" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G70" t="s">
         <v>41</v>
@@ -4882,10 +4883,10 @@
         <v>59</v>
       </c>
       <c r="N70" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O70" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P70" t="s">
         <v>32</v>
@@ -4894,45 +4895,45 @@
         <v>33</v>
       </c>
       <c r="Y70" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>11377</v>
-      </c>
-      <c r="C71">
-        <v>11377</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" t="s">
+        <v>37</v>
       </c>
       <c r="D71">
-        <v>11377</v>
+        <v>10763</v>
       </c>
       <c r="E71" t="s">
         <v>26</v>
       </c>
       <c r="F71" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G71" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H71" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="I71" t="s">
         <v>29</v>
       </c>
       <c r="J71" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="K71" t="s">
         <v>28</v>
       </c>
       <c r="L71">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="M71">
-        <v>35</v>
+        <v>775</v>
       </c>
       <c r="N71" t="s">
         <v>39</v>
@@ -4943,64 +4944,49 @@
       <c r="P71" t="s">
         <v>32</v>
       </c>
-      <c r="Q71">
-        <v>1170</v>
-      </c>
-      <c r="R71" t="s">
-        <v>73</v>
-      </c>
-      <c r="S71">
-        <v>364</v>
-      </c>
-      <c r="T71">
-        <v>0.5</v>
-      </c>
-      <c r="U71" t="s">
-        <v>47</v>
-      </c>
       <c r="X71" t="s">
         <v>33</v>
       </c>
       <c r="Y71" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>11377</v>
-      </c>
-      <c r="C72">
-        <v>11377</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" t="s">
+        <v>37</v>
       </c>
       <c r="D72">
-        <v>11377</v>
+        <v>10763</v>
       </c>
       <c r="E72" t="s">
         <v>26</v>
       </c>
       <c r="F72" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G72" t="s">
         <v>27</v>
       </c>
       <c r="H72" t="s">
-        <v>71</v>
-      </c>
-      <c r="I72" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I72">
+        <v>2199</v>
       </c>
       <c r="J72" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="K72" t="s">
         <v>28</v>
       </c>
       <c r="L72">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="M72">
-        <v>456</v>
+        <v>360</v>
       </c>
       <c r="N72" t="s">
         <v>39</v>
@@ -5011,64 +4997,49 @@
       <c r="P72" t="s">
         <v>32</v>
       </c>
-      <c r="Q72">
-        <v>3090</v>
-      </c>
-      <c r="R72" t="s">
-        <v>76</v>
-      </c>
-      <c r="S72">
-        <v>968</v>
-      </c>
-      <c r="T72">
-        <v>0.5</v>
-      </c>
-      <c r="U72" t="s">
-        <v>47</v>
-      </c>
       <c r="X72" t="s">
         <v>33</v>
       </c>
       <c r="Y72" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>11377</v>
-      </c>
-      <c r="C73">
-        <v>11377</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" t="s">
+        <v>37</v>
       </c>
       <c r="D73">
-        <v>11377</v>
+        <v>10763</v>
       </c>
       <c r="E73" t="s">
         <v>26</v>
       </c>
       <c r="F73" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G73" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="H73" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="I73" t="s">
         <v>29</v>
       </c>
       <c r="J73" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="K73" t="s">
         <v>28</v>
       </c>
       <c r="L73">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="M73">
-        <v>230</v>
+        <v>59</v>
       </c>
       <c r="N73" t="s">
         <v>39</v>
@@ -5079,37 +5050,22 @@
       <c r="P73" t="s">
         <v>32</v>
       </c>
-      <c r="Q73">
-        <v>1075</v>
-      </c>
-      <c r="R73" t="s">
-        <v>78</v>
-      </c>
-      <c r="S73">
-        <v>200</v>
-      </c>
-      <c r="T73">
-        <v>0.5</v>
-      </c>
-      <c r="U73" t="s">
-        <v>47</v>
-      </c>
       <c r="X73" t="s">
         <v>33</v>
       </c>
       <c r="Y73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>36</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>11377</v>
       </c>
       <c r="C74">
         <v>11377</v>
       </c>
       <c r="D74">
-        <v>10763</v>
+        <v>11377</v>
       </c>
       <c r="E74" t="s">
         <v>26</v>
@@ -5118,154 +5074,199 @@
         <v>49</v>
       </c>
       <c r="G74" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="H74" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I74" t="s">
         <v>29</v>
       </c>
       <c r="J74" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="K74" t="s">
         <v>28</v>
       </c>
       <c r="L74">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M74">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="N74" t="s">
         <v>39</v>
       </c>
       <c r="O74" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P74" t="s">
         <v>32</v>
       </c>
+      <c r="Q74">
+        <v>1170</v>
+      </c>
+      <c r="R74" t="s">
+        <v>73</v>
+      </c>
+      <c r="S74">
+        <v>364</v>
+      </c>
+      <c r="T74">
+        <v>0.5</v>
+      </c>
+      <c r="U74" t="s">
+        <v>47</v>
+      </c>
       <c r="X74" t="s">
         <v>33</v>
       </c>
       <c r="Y74" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C75" t="s">
-        <v>82</v>
-      </c>
-      <c r="D75" t="s">
-        <v>83</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>11377</v>
+      </c>
+      <c r="C75">
+        <v>11377</v>
+      </c>
+      <c r="D75">
+        <v>11377</v>
       </c>
       <c r="E75" t="s">
         <v>26</v>
       </c>
       <c r="F75" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G75" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="H75" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="I75" t="s">
         <v>29</v>
       </c>
       <c r="J75" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="K75" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="L75">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="M75">
-        <v>59</v>
+        <v>456</v>
       </c>
       <c r="N75" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O75" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="P75" t="s">
         <v>32</v>
       </c>
+      <c r="Q75">
+        <v>3090</v>
+      </c>
+      <c r="R75" t="s">
+        <v>76</v>
+      </c>
+      <c r="S75">
+        <v>968</v>
+      </c>
+      <c r="T75">
+        <v>0.5</v>
+      </c>
+      <c r="U75" t="s">
+        <v>47</v>
+      </c>
       <c r="X75" t="s">
         <v>33</v>
       </c>
       <c r="Y75" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>36</v>
-      </c>
-      <c r="C76" t="s">
-        <v>82</v>
-      </c>
-      <c r="D76" t="s">
-        <v>83</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>11377</v>
+      </c>
+      <c r="C76">
+        <v>11377</v>
+      </c>
+      <c r="D76">
+        <v>11377</v>
       </c>
       <c r="E76" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F76" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="G76" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="H76" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="I76" t="s">
         <v>29</v>
       </c>
       <c r="J76" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="K76" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="L76">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="M76">
-        <v>59</v>
+        <v>230</v>
       </c>
       <c r="N76" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O76" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="P76" t="s">
         <v>32</v>
       </c>
+      <c r="Q76">
+        <v>1075</v>
+      </c>
+      <c r="R76" t="s">
+        <v>78</v>
+      </c>
+      <c r="S76">
+        <v>200</v>
+      </c>
+      <c r="T76">
+        <v>0.5</v>
+      </c>
+      <c r="U76" t="s">
+        <v>47</v>
+      </c>
       <c r="X76" t="s">
         <v>33</v>
       </c>
       <c r="Y76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>36</v>
       </c>
-      <c r="B77" t="s">
-        <v>37</v>
+      <c r="C77">
+        <v>11377</v>
       </c>
       <c r="D77">
         <v>10763</v>
@@ -5277,7 +5278,7 @@
         <v>49</v>
       </c>
       <c r="G77" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="H77" t="s">
         <v>80</v>
@@ -5298,11 +5299,11 @@
         <v>87</v>
       </c>
       <c r="N77" t="s">
+        <v>39</v>
+      </c>
+      <c r="O77" t="s">
         <v>30</v>
       </c>
-      <c r="O77" t="s">
-        <v>31</v>
-      </c>
       <c r="P77" t="s">
         <v>32</v>
       </c>
@@ -5310,30 +5311,30 @@
         <v>33</v>
       </c>
       <c r="Y77" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>11377</v>
-      </c>
-      <c r="C78">
-        <v>11377</v>
-      </c>
-      <c r="D78">
-        <v>11377</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>36</v>
+      </c>
+      <c r="C78" t="s">
+        <v>82</v>
+      </c>
+      <c r="D78" t="s">
+        <v>83</v>
       </c>
       <c r="E78" t="s">
         <v>26</v>
       </c>
       <c r="F78" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G78" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="H78" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="I78" t="s">
         <v>29</v>
@@ -5342,7 +5343,7 @@
         <v>28</v>
       </c>
       <c r="K78" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="L78">
         <v>2</v>
@@ -5351,81 +5352,75 @@
         <v>59</v>
       </c>
       <c r="N78" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O78" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="P78" t="s">
         <v>32</v>
       </c>
-      <c r="V78" t="s">
-        <v>65</v>
-      </c>
       <c r="X78" t="s">
         <v>33</v>
       </c>
       <c r="Y78" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>11377</v>
-      </c>
-      <c r="C79">
-        <v>11377</v>
-      </c>
-      <c r="D79">
-        <v>11377</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79" t="s">
+        <v>82</v>
+      </c>
+      <c r="D79" t="s">
+        <v>83</v>
       </c>
       <c r="E79" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="F79" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G79" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="H79" t="s">
-        <v>28</v>
-      </c>
-      <c r="I79">
-        <v>2199</v>
+        <v>85</v>
+      </c>
+      <c r="I79" t="s">
+        <v>29</v>
       </c>
       <c r="J79" t="s">
         <v>28</v>
       </c>
       <c r="K79" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="L79">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="M79">
-        <v>259</v>
+        <v>59</v>
       </c>
       <c r="N79" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O79" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="P79" t="s">
         <v>32</v>
       </c>
-      <c r="V79" t="s">
-        <v>38</v>
-      </c>
       <c r="X79" t="s">
         <v>33</v>
       </c>
       <c r="Y79" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>36</v>
       </c>
@@ -5442,10 +5437,10 @@
         <v>49</v>
       </c>
       <c r="G80" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H80" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="I80" t="s">
         <v>29</v>
@@ -5457,16 +5452,16 @@
         <v>28</v>
       </c>
       <c r="L80">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="M80">
-        <v>775</v>
+        <v>87</v>
       </c>
       <c r="N80" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O80" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P80" t="s">
         <v>32</v>
@@ -5475,24 +5470,24 @@
         <v>33</v>
       </c>
       <c r="Y80" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>36</v>
-      </c>
-      <c r="B81" t="s">
-        <v>37</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>11377</v>
+      </c>
+      <c r="C81">
+        <v>11377</v>
       </c>
       <c r="D81">
-        <v>10763</v>
+        <v>11377</v>
       </c>
       <c r="E81" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="F81" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G81" t="s">
         <v>35</v>
@@ -5510,10 +5505,10 @@
         <v>28</v>
       </c>
       <c r="L81">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="M81">
-        <v>775</v>
+        <v>59</v>
       </c>
       <c r="N81" t="s">
         <v>39</v>
@@ -5524,28 +5519,31 @@
       <c r="P81" t="s">
         <v>32</v>
       </c>
+      <c r="V81" t="s">
+        <v>65</v>
+      </c>
       <c r="X81" t="s">
         <v>33</v>
       </c>
       <c r="Y81" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>36</v>
-      </c>
-      <c r="B82" t="s">
-        <v>37</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>11377</v>
+      </c>
+      <c r="C82">
+        <v>11377</v>
       </c>
       <c r="D82">
-        <v>10763</v>
+        <v>11377</v>
       </c>
       <c r="E82" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="F82" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G82" t="s">
         <v>27</v>
@@ -5563,10 +5561,10 @@
         <v>28</v>
       </c>
       <c r="L82">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="M82">
-        <v>360</v>
+        <v>259</v>
       </c>
       <c r="N82" t="s">
         <v>39</v>
@@ -5577,14 +5575,17 @@
       <c r="P82" t="s">
         <v>32</v>
       </c>
+      <c r="V82" t="s">
+        <v>38</v>
+      </c>
       <c r="X82" t="s">
         <v>33</v>
       </c>
       <c r="Y82" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>36</v>
       </c>
@@ -5595,13 +5596,13 @@
         <v>10763</v>
       </c>
       <c r="E83" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="F83" t="s">
         <v>49</v>
       </c>
       <c r="G83" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H83" t="s">
         <v>28</v>
@@ -5616,10 +5617,10 @@
         <v>28</v>
       </c>
       <c r="L83">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="M83">
-        <v>59</v>
+        <v>775</v>
       </c>
       <c r="N83" t="s">
         <v>39</v>
@@ -5634,24 +5635,24 @@
         <v>33</v>
       </c>
       <c r="Y83" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A84">
-        <v>11377</v>
-      </c>
-      <c r="C84">
-        <v>11377</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>36</v>
+      </c>
+      <c r="B84" t="s">
+        <v>37</v>
       </c>
       <c r="D84">
-        <v>11377</v>
+        <v>10763</v>
       </c>
       <c r="E84" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="F84" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G84" t="s">
         <v>35</v>
@@ -5675,36 +5676,33 @@
         <v>775</v>
       </c>
       <c r="N84" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O84" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P84" t="s">
         <v>32</v>
       </c>
-      <c r="W84">
+      <c r="X84" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>36</v>
+      </c>
+      <c r="B85" t="s">
+        <v>37</v>
+      </c>
+      <c r="D85">
         <v>10763</v>
       </c>
-      <c r="X84" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y84" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A85">
-        <v>11377</v>
-      </c>
-      <c r="C85">
-        <v>11029</v>
-      </c>
-      <c r="D85">
-        <v>10757</v>
-      </c>
       <c r="E85" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="F85" t="s">
         <v>49</v>
@@ -5716,40 +5714,214 @@
         <v>28</v>
       </c>
       <c r="I85">
+        <v>2199</v>
+      </c>
+      <c r="J85" t="s">
+        <v>28</v>
+      </c>
+      <c r="K85" t="s">
+        <v>28</v>
+      </c>
+      <c r="L85">
+        <v>8</v>
+      </c>
+      <c r="M85">
+        <v>360</v>
+      </c>
+      <c r="N85" t="s">
+        <v>39</v>
+      </c>
+      <c r="O85" t="s">
+        <v>28</v>
+      </c>
+      <c r="P85" t="s">
+        <v>32</v>
+      </c>
+      <c r="X85" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>36</v>
+      </c>
+      <c r="B86" t="s">
+        <v>37</v>
+      </c>
+      <c r="D86">
+        <v>10763</v>
+      </c>
+      <c r="E86" t="s">
+        <v>91</v>
+      </c>
+      <c r="F86" t="s">
+        <v>49</v>
+      </c>
+      <c r="G86" t="s">
+        <v>41</v>
+      </c>
+      <c r="H86" t="s">
+        <v>28</v>
+      </c>
+      <c r="I86" t="s">
+        <v>29</v>
+      </c>
+      <c r="J86" t="s">
+        <v>28</v>
+      </c>
+      <c r="K86" t="s">
+        <v>28</v>
+      </c>
+      <c r="L86">
+        <v>2</v>
+      </c>
+      <c r="M86">
+        <v>59</v>
+      </c>
+      <c r="N86" t="s">
+        <v>39</v>
+      </c>
+      <c r="O86" t="s">
+        <v>28</v>
+      </c>
+      <c r="P86" t="s">
+        <v>32</v>
+      </c>
+      <c r="X86" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>11377</v>
+      </c>
+      <c r="C87">
+        <v>11377</v>
+      </c>
+      <c r="D87">
+        <v>11377</v>
+      </c>
+      <c r="E87" t="s">
+        <v>26</v>
+      </c>
+      <c r="F87" t="s">
+        <v>61</v>
+      </c>
+      <c r="G87" t="s">
+        <v>35</v>
+      </c>
+      <c r="H87" t="s">
+        <v>28</v>
+      </c>
+      <c r="I87" t="s">
+        <v>29</v>
+      </c>
+      <c r="J87" t="s">
+        <v>28</v>
+      </c>
+      <c r="K87" t="s">
+        <v>28</v>
+      </c>
+      <c r="L87">
+        <v>13</v>
+      </c>
+      <c r="M87">
+        <v>775</v>
+      </c>
+      <c r="N87" t="s">
+        <v>30</v>
+      </c>
+      <c r="O87" t="s">
+        <v>31</v>
+      </c>
+      <c r="P87" t="s">
+        <v>32</v>
+      </c>
+      <c r="W87">
+        <v>10763</v>
+      </c>
+      <c r="X87" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y87" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:25" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>11377</v>
+      </c>
+      <c r="C88">
+        <v>11029</v>
+      </c>
+      <c r="D88">
+        <v>10757</v>
+      </c>
+      <c r="E88" t="s">
+        <v>26</v>
+      </c>
+      <c r="F88" t="s">
+        <v>49</v>
+      </c>
+      <c r="G88" t="s">
+        <v>27</v>
+      </c>
+      <c r="H88" t="s">
+        <v>28</v>
+      </c>
+      <c r="I88">
         <v>2300</v>
       </c>
-      <c r="J85" t="s">
-        <v>28</v>
-      </c>
-      <c r="K85" t="s">
-        <v>28</v>
-      </c>
-      <c r="L85">
+      <c r="J88" t="s">
+        <v>28</v>
+      </c>
+      <c r="K88" t="s">
+        <v>28</v>
+      </c>
+      <c r="L88">
         <v>5</v>
       </c>
-      <c r="M85">
+      <c r="M88">
         <v>250</v>
       </c>
-      <c r="N85" t="s">
+      <c r="N88" t="s">
         <v>30</v>
       </c>
-      <c r="O85" t="s">
+      <c r="O88" t="s">
         <v>31</v>
       </c>
-      <c r="P85" t="s">
-        <v>32</v>
-      </c>
-      <c r="W85">
+      <c r="P88" t="s">
+        <v>32</v>
+      </c>
+      <c r="W88">
         <v>10763</v>
       </c>
-      <c r="X85" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y85" t="s">
+      <c r="X88" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y88" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Y88" xr:uid="{C13A9B56-5E6E-4A35-9DD7-E48E0C4AA254}">
+    <filterColumn colId="24">
+      <filters>
+        <filter val="LTE001_ACC_00001"/>
+        <filter val="LTE001_ACC_00002"/>
+        <filter val="LTE001_ACC_00003"/>
+        <filter val="LTE001_ACC_00004"/>
+        <filter val="LTE001_ACC_00005"/>
+        <filter val="LTE001_ACC_00007"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated chrome, added LTE testcase
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-vkaushal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FF37F6-4FF8-4585-99BB-DE5D32597207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D556BD97-ABB8-40BB-9663-ADA075854543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" activeTab="1" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" activeTab="3" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="92">
   <si>
     <t>AgentCode</t>
   </si>
@@ -269,9 +269,6 @@
     <t>DFW</t>
   </si>
   <si>
-    <t>LTE001_ACC_00003</t>
-  </si>
-  <si>
     <t>UN2807</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
   </si>
   <si>
     <t>Nitrogen, refrigerated liquid</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00004</t>
   </si>
   <si>
     <t>LTE001_ACC_00005</t>
@@ -976,7 +970,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1029,7 +1023,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1082,7 +1076,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1239,7 +1233,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1292,7 +1286,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1345,7 +1339,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1521,7 +1515,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1589,7 +1583,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1657,7 +1651,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1814,7 +1808,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1929,7 +1923,7 @@
         <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1971,7 +1965,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1982,7 +1976,7 @@
         <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
@@ -2024,7 +2018,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2181,7 +2175,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2342,7 +2336,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2398,7 +2392,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2555,7 +2549,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2712,7 +2706,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2765,7 +2759,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -2818,7 +2812,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2979,7 +2973,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -3035,7 +3029,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3047,7 +3041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02740B3-88E5-4DDF-8354-11DFF949E13D}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -3259,748 +3253,655 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55333C5B-4CB8-438D-AA05-F854870A7A77}">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="17" max="17" width="28.42578125" customWidth="1"/>
-    <col min="18" max="18" width="17" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="28.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" customWidth="1"/>
+    <col min="20" max="20" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2">
+        <v>8000</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2">
+        <v>0.5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>65</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3">
+        <v>1845</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3">
+        <v>954</v>
+      </c>
+      <c r="S3">
+        <v>0.5</v>
+      </c>
+      <c r="T3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>99</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4">
+        <v>3110</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4">
+        <v>570</v>
+      </c>
+      <c r="S4">
+        <v>0.5</v>
+      </c>
+      <c r="T4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11377</v>
+      </c>
+      <c r="B5">
+        <v>11377</v>
+      </c>
+      <c r="C5">
+        <v>11377</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L5">
+        <v>30</v>
+      </c>
+      <c r="M5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5">
+        <v>2807</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R5" s="2">
+        <v>953</v>
+      </c>
+      <c r="S5">
+        <v>0.5</v>
+      </c>
+      <c r="T5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11377</v>
+      </c>
+      <c r="B6">
+        <v>11377</v>
+      </c>
+      <c r="C6">
+        <v>11377</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>30</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="L6">
+        <v>65</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" t="s">
         <v>22</v>
       </c>
-      <c r="Q2">
-        <v>8000</v>
-      </c>
-      <c r="R2" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T2">
+      <c r="P6">
+        <v>1977</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6">
+        <v>202</v>
+      </c>
+      <c r="S6">
         <v>0.5</v>
       </c>
-      <c r="U2" t="s">
+      <c r="T6" t="s">
         <v>31</v>
       </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>65</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3">
-        <v>1845</v>
-      </c>
-      <c r="R3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3">
-        <v>954</v>
-      </c>
-      <c r="T3">
-        <v>0.5</v>
-      </c>
-      <c r="U3" t="s">
-        <v>31</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>11377</v>
-      </c>
-      <c r="C4">
-        <v>11377</v>
-      </c>
-      <c r="D4">
-        <v>11377</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4">
-        <v>3</v>
-      </c>
-      <c r="M4">
-        <v>99</v>
-      </c>
-      <c r="N4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4">
-        <v>3110</v>
-      </c>
-      <c r="R4" t="s">
-        <v>32</v>
-      </c>
-      <c r="S4">
-        <v>570</v>
-      </c>
-      <c r="T4">
-        <v>0.5</v>
-      </c>
-      <c r="U4" t="s">
-        <v>31</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>11377</v>
-      </c>
-      <c r="C5">
-        <v>11377</v>
-      </c>
-      <c r="D5">
-        <v>11377</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>72</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>30</v>
-      </c>
-      <c r="N5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5">
-        <v>2807</v>
-      </c>
-      <c r="R5" t="s">
-        <v>73</v>
-      </c>
-      <c r="S5" s="2">
-        <v>953</v>
-      </c>
-      <c r="T5">
-        <v>0.5</v>
-      </c>
-      <c r="U5" t="s">
-        <v>31</v>
-      </c>
-      <c r="X5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>11377</v>
-      </c>
-      <c r="C6">
-        <v>11377</v>
-      </c>
-      <c r="D6">
-        <v>11377</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" t="s">
-        <v>74</v>
-      </c>
-      <c r="K6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6">
-        <v>2</v>
-      </c>
-      <c r="M6">
-        <v>65</v>
-      </c>
-      <c r="N6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O6" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q6">
-        <v>1977</v>
-      </c>
-      <c r="R6" t="s">
-        <v>75</v>
-      </c>
-      <c r="S6">
-        <v>202</v>
-      </c>
-      <c r="T6">
-        <v>0.5</v>
-      </c>
-      <c r="U6" t="s">
-        <v>31</v>
-      </c>
-      <c r="X6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="S8" s="2"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="S12" s="2"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="S13" s="2"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="S14" s="2"/>
-    </row>
-    <row r="17" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S17" s="2"/>
-    </row>
-    <row r="20" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S20" s="2"/>
-    </row>
-    <row r="22" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S22" s="2"/>
-    </row>
-    <row r="23" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S23" s="2"/>
-    </row>
-    <row r="24" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S24" s="2"/>
-    </row>
-    <row r="25" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S25" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R8" s="2"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R14" s="2"/>
+    </row>
+    <row r="17" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R17" s="2"/>
+    </row>
+    <row r="20" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R20" s="2"/>
+    </row>
+    <row r="22" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE920C76-3A37-4057-8B20-893482492082}">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>775</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>360</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>13</v>
-      </c>
-      <c r="M2">
-        <v>775</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="L4">
+        <v>55</v>
+      </c>
+      <c r="M4" t="s">
         <v>20</v>
       </c>
-      <c r="O2" t="s">
+      <c r="N4" t="s">
         <v>21</v>
       </c>
-      <c r="P2" t="s">
+      <c r="O4" t="s">
         <v>22</v>
       </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>8</v>
-      </c>
-      <c r="M3">
-        <v>360</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>11377</v>
-      </c>
-      <c r="C4">
-        <v>11377</v>
-      </c>
-      <c r="D4">
-        <v>11377</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>55</v>
-      </c>
-      <c r="N4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="I5" s="1"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="I7" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4159,7 +4060,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4212,7 +4113,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -4265,7 +4166,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -4423,7 +4324,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4476,7 +4377,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -4529,7 +4430,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -4582,7 +4483,7 @@
         <v>23</v>
       </c>
       <c r="Y5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -4635,7 +4536,7 @@
         <v>23</v>
       </c>
       <c r="Y6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -4688,7 +4589,7 @@
         <v>23</v>
       </c>
       <c r="Y7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -4849,7 +4750,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4905,7 +4806,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -4961,7 +4862,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -4981,7 +4882,7 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
@@ -5017,7 +4918,7 @@
         <v>23</v>
       </c>
       <c r="Y5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -5174,7 +5075,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -5227,7 +5128,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -5280,7 +5181,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -5440,7 +5341,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -5496,7 +5397,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added  trait field and lte testcases
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-vkaushal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB37286-A929-4187-8836-8F3B84317EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4AC13D-200B-4D9C-9257-7EF0487B3707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" firstSheet="4" activeTab="4" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" firstSheet="7" activeTab="7" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="87">
   <si>
     <t>AgentCode</t>
   </si>
@@ -283,18 +283,6 @@
   </si>
   <si>
     <t>PET CONNECT</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00009</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00010</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00011</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00012</t>
   </si>
   <si>
     <t>LTE001_ACC_00015</t>
@@ -705,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15025949-10D9-4C1B-9506-C6E07A0B91EB}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,213 +809,163 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C9544C-A3E8-4087-8CA1-7B6068AB4469}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="5" max="6" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="L2">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>2199</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>36</v>
+      </c>
+      <c r="L3">
+        <v>259</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2">
-        <v>59</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="V2" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <v>2199</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>36</v>
-      </c>
-      <c r="M3">
-        <v>259</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V3" t="s">
-        <v>27</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1037,260 +975,199 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588B3A75-C7DB-40C6-BCDF-882DAD4C0277}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>775</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>2199</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>360</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>13</v>
-      </c>
-      <c r="M2">
-        <v>775</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <v>2199</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>8</v>
-      </c>
-      <c r="M3">
-        <v>360</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>11377</v>
-      </c>
-      <c r="C4">
-        <v>11377</v>
-      </c>
-      <c r="D4">
-        <v>11377</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
       <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
         <v>59</v>
       </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
       <c r="N4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1300,27 +1177,26 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F85EB7-D4FE-4731-A89B-6B56A2672E3B}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1328,232 +1204,172 @@
         <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="D2">
+      <c r="C2">
         <v>10763</v>
       </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
-        <v>18</v>
+      <c r="K2">
+        <v>13</v>
       </c>
       <c r="L2">
-        <v>13</v>
-      </c>
-      <c r="M2">
         <v>775</v>
       </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
       <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <v>10763</v>
       </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="H3">
         <v>2199</v>
       </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
       <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" t="s">
-        <v>18</v>
+      <c r="K3">
+        <v>8</v>
       </c>
       <c r="L3">
-        <v>8</v>
-      </c>
-      <c r="M3">
         <v>360</v>
       </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
       <c r="N3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>10763</v>
       </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" t="s">
-        <v>18</v>
+      <c r="K4">
+        <v>2</v>
       </c>
       <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
         <v>59</v>
       </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
       <c r="N4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1729,7 +1545,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1797,7 +1613,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1865,7 +1681,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2022,7 +1838,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2137,7 +1953,7 @@
         <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -2179,7 +1995,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2190,7 +2006,7 @@
         <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
@@ -2232,7 +2048,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2389,7 +2205,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2550,7 +2366,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2606,7 +2422,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2763,7 +2579,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2920,7 +2736,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2973,7 +2789,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -3026,7 +2842,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3401,7 +3217,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -3457,7 +3273,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -4125,9 +3941,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA38A178-4DE0-471C-BD3C-CC9822D93DCD}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -4339,7 +4155,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -4356,7 +4172,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -4735,8 +4551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A641F-CDF5-42AA-90C2-89A89CF0D81F}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4844,10 +4660,10 @@
         <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O2" t="s">
         <v>22</v>
@@ -4897,10 +4713,10 @@
         <v>324</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O3" t="s">
         <v>22</v>
@@ -4950,10 +4766,10 @@
         <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O4" t="s">
         <v>22</v>
@@ -5003,10 +4819,10 @@
         <v>59</v>
       </c>
       <c r="M5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O5" t="s">
         <v>22</v>
@@ -5026,260 +4842,199 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0702AE-AE2A-4040-B020-48654513E736}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>775</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L3">
+        <v>200</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>13</v>
-      </c>
-      <c r="M2">
-        <v>775</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="L4">
+        <v>840</v>
+      </c>
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>6</v>
-      </c>
-      <c r="M3">
-        <v>200</v>
-      </c>
-      <c r="N3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>11377</v>
-      </c>
-      <c r="C4">
-        <v>11377</v>
-      </c>
-      <c r="D4">
-        <v>11377</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4">
-        <v>8</v>
-      </c>
-      <c r="M4">
-        <v>840</v>
-      </c>
       <c r="N4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 3 more OPR344 scenarios and added tags above each tests
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-vkaushal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D556BD97-ABB8-40BB-9663-ADA075854543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB37286-A929-4187-8836-8F3B84317EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" activeTab="3" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" firstSheet="4" activeTab="4" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -18,20 +18,21 @@
     <sheet name="LTE001_ACC_00003" sheetId="3" r:id="rId3"/>
     <sheet name="LTE001_ACC_00004" sheetId="4" r:id="rId4"/>
     <sheet name="LTE001_ACC_00005" sheetId="5" r:id="rId5"/>
-    <sheet name="LTE001_ACC_00007" sheetId="6" r:id="rId6"/>
-    <sheet name="LTE001_ACC_00008" sheetId="7" r:id="rId7"/>
-    <sheet name="LTE001_ACC_00009" sheetId="8" r:id="rId8"/>
-    <sheet name="LTE001_ACC_00010" sheetId="9" r:id="rId9"/>
-    <sheet name="LTE001_ACC_00011" sheetId="10" r:id="rId10"/>
-    <sheet name="LTE001_ACC_00012" sheetId="11" r:id="rId11"/>
-    <sheet name="LTE001_ACC_00015" sheetId="12" r:id="rId12"/>
-    <sheet name="LTE001_ACC_00016" sheetId="13" r:id="rId13"/>
-    <sheet name="LTE001_ACC_00017" sheetId="14" r:id="rId14"/>
-    <sheet name="LTE001_ACC_00019" sheetId="15" r:id="rId15"/>
-    <sheet name="LTE001_ACC_00021" sheetId="16" r:id="rId16"/>
-    <sheet name="LTE001_ACC_00023" sheetId="17" r:id="rId17"/>
-    <sheet name="LTE001_ACC_00024" sheetId="18" r:id="rId18"/>
-    <sheet name="LTE001_ACC_00028" sheetId="19" r:id="rId19"/>
+    <sheet name="LTE001_ACC_00006" sheetId="21" r:id="rId6"/>
+    <sheet name="LTE001_ACC_00007" sheetId="6" r:id="rId7"/>
+    <sheet name="LTE001_ACC_00008" sheetId="7" r:id="rId8"/>
+    <sheet name="LTE001_ACC_00009" sheetId="8" r:id="rId9"/>
+    <sheet name="LTE001_ACC_00010" sheetId="9" r:id="rId10"/>
+    <sheet name="LTE001_ACC_00011" sheetId="10" r:id="rId11"/>
+    <sheet name="LTE001_ACC_00012" sheetId="11" r:id="rId12"/>
+    <sheet name="LTE001_ACC_00015" sheetId="12" r:id="rId13"/>
+    <sheet name="LTE001_ACC_00016" sheetId="13" r:id="rId14"/>
+    <sheet name="LTE001_ACC_00017" sheetId="14" r:id="rId15"/>
+    <sheet name="LTE001_ACC_00019" sheetId="15" r:id="rId16"/>
+    <sheet name="LTE001_ACC_00021" sheetId="16" r:id="rId17"/>
+    <sheet name="LTE001_ACC_00023" sheetId="17" r:id="rId18"/>
+    <sheet name="LTE001_ACC_00024" sheetId="18" r:id="rId19"/>
+    <sheet name="LTE001_ACC_00028" sheetId="19" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="91">
   <si>
     <t>AgentCode</t>
   </si>
@@ -281,15 +282,6 @@
     <t>Nitrogen, refrigerated liquid</t>
   </si>
   <si>
-    <t>LTE001_ACC_00005</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00007</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00008</t>
-  </si>
-  <si>
     <t>PET CONNECT</t>
   </si>
   <si>
@@ -330,6 +322,12 @@
   </si>
   <si>
     <t>LTE001_ACC_00028</t>
+  </si>
+  <si>
+    <t>PreBookedAWB</t>
+  </si>
+  <si>
+    <t>027-30077655</t>
   </si>
 </sst>
 </file>
@@ -822,6 +820,222 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C9544C-A3E8-4087-8CA1-7B6068AB4469}">
+  <dimension ref="A1:Y3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="5" max="6" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" t="s">
+        <v>68</v>
+      </c>
+      <c r="X1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2">
+        <v>11377</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>59</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3">
+        <v>11377</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>2199</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3">
+        <v>36</v>
+      </c>
+      <c r="M3">
+        <v>259</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588B3A75-C7DB-40C6-BCDF-882DAD4C0277}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -970,7 +1184,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1023,7 +1237,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1076,7 +1290,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1084,7 +1298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F85EB7-D4FE-4731-A89B-6B56A2672E3B}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -1233,7 +1447,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1286,7 +1500,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1339,7 +1553,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1348,7 +1562,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E9B1A2-8828-4F98-87B5-7CAF91123FE0}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -1515,7 +1729,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1583,7 +1797,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1651,7 +1865,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1660,7 +1874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283541C0-DDFC-48C8-A86D-03373D5A40BC}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
@@ -1808,7 +2022,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1816,7 +2030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52D668D-AC07-43A4-9449-F9469656E50D}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
@@ -1923,7 +2137,7 @@
         <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1965,7 +2179,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1976,7 +2190,7 @@
         <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
@@ -2018,7 +2232,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2026,7 +2240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214D453D-CE5B-419D-B0CA-C2374C08FCBA}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
@@ -2175,7 +2389,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2183,7 +2397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6658BEBD-BE9E-40E4-8B04-B10FCCEDE4E2}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
@@ -2336,7 +2550,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2392,7 +2606,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2400,7 +2614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42907D3-7B5D-45F4-B15C-E3ED5A7006FE}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
@@ -2549,7 +2763,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2557,7 +2771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1BD66A-844E-4EDA-88D7-6B09C94784A4}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -2706,7 +2920,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2759,7 +2973,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -2812,224 +3026,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8C0BE7-2417-43A3-B581-D983787A9A47}">
-  <dimension ref="A1:Y3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Y3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>13</v>
-      </c>
-      <c r="M2">
-        <v>775</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="W2">
-        <v>10763</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11029</v>
-      </c>
-      <c r="D3">
-        <v>10757</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <v>2300</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>5</v>
-      </c>
-      <c r="M3">
-        <v>250</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="W3">
-        <v>10763</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3244,6 +3241,223 @@
       </c>
       <c r="O4" t="s">
         <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8C0BE7-2417-43A3-B581-D983787A9A47}">
+  <dimension ref="A1:Y3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:Y3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" t="s">
+        <v>68</v>
+      </c>
+      <c r="X1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2">
+        <v>11377</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2">
+        <v>13</v>
+      </c>
+      <c r="M2">
+        <v>775</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2">
+        <v>10763</v>
+      </c>
+      <c r="X2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11029</v>
+      </c>
+      <c r="D3">
+        <v>10757</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>2300</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>250</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W3">
+        <v>10763</v>
+      </c>
+      <c r="X3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3695,8 +3909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE920C76-3A37-4057-8B20-893482492082}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3913,260 +4127,198 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA38A178-4DE0-471C-BD3C-CC9822D93DCD}">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
-    <col min="25" max="25" width="8.5703125" customWidth="1"/>
-    <col min="26" max="26" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="L3">
+        <v>600</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E4" t="s">
         <v>38</v>
       </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>100</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
+        <v>20</v>
+      </c>
+      <c r="L4">
+        <v>750</v>
+      </c>
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>8</v>
-      </c>
-      <c r="M3">
-        <v>600</v>
-      </c>
-      <c r="N3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>11377</v>
-      </c>
-      <c r="C4">
-        <v>11377</v>
-      </c>
-      <c r="D4">
-        <v>11377</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4">
-        <v>20</v>
-      </c>
-      <c r="M4">
-        <v>750</v>
-      </c>
       <c r="N4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -4176,420 +4328,47 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1051281-76C6-44DD-9FC2-1F77E64E8898}">
-  <dimension ref="A1:Y7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D71B933-D35A-4F10-8F8D-DB21B7A241A8}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>20</v>
-      </c>
-      <c r="M2">
-        <v>750</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" t="s">
         <v>22</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>18</v>
-      </c>
-      <c r="M3">
-        <v>360</v>
-      </c>
-      <c r="N3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>11377</v>
-      </c>
-      <c r="C4">
-        <v>11377</v>
-      </c>
-      <c r="D4">
-        <v>11377</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>55</v>
-      </c>
-      <c r="N4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>11377</v>
-      </c>
-      <c r="C5">
-        <v>11377</v>
-      </c>
-      <c r="D5">
-        <v>11377</v>
-      </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5">
-        <v>20</v>
-      </c>
-      <c r="M5">
-        <v>750</v>
-      </c>
-      <c r="N5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" t="s">
-        <v>22</v>
-      </c>
-      <c r="X5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>11377</v>
-      </c>
-      <c r="C6">
-        <v>11377</v>
-      </c>
-      <c r="D6">
-        <v>11377</v>
-      </c>
-      <c r="E6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6">
-        <v>18</v>
-      </c>
-      <c r="M6">
-        <v>360</v>
-      </c>
-      <c r="N6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O6" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" t="s">
-        <v>22</v>
-      </c>
-      <c r="X6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>11377</v>
-      </c>
-      <c r="C7">
-        <v>11377</v>
-      </c>
-      <c r="D7">
-        <v>11377</v>
-      </c>
-      <c r="E7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7">
-        <v>2</v>
-      </c>
-      <c r="M7">
-        <v>55</v>
-      </c>
-      <c r="N7" t="s">
-        <v>25</v>
-      </c>
-      <c r="O7" t="s">
-        <v>18</v>
-      </c>
-      <c r="P7" t="s">
-        <v>22</v>
-      </c>
-      <c r="X7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -4598,327 +4377,353 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A641F-CDF5-42AA-90C2-89A89CF0D81F}">
-  <dimension ref="A1:Y5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1051281-76C6-44DD-9FC2-1F77E64E8898}">
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+      <c r="L2">
+        <v>750</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>18</v>
+      </c>
+      <c r="L3">
+        <v>360</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2">
-        <v>59</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="L4">
+        <v>55</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" t="s">
         <v>22</v>
       </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <v>2199</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>12</v>
-      </c>
-      <c r="M3">
-        <v>324</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>11377</v>
-      </c>
-      <c r="C4">
-        <v>11377</v>
-      </c>
-      <c r="D4">
-        <v>11377</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>59</v>
-      </c>
-      <c r="N4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="V4">
-        <v>1</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11377</v>
       </c>
+      <c r="B5">
+        <v>11377</v>
+      </c>
       <c r="C5">
         <v>11377</v>
       </c>
-      <c r="D5">
-        <v>11377</v>
+      <c r="D5" t="s">
+        <v>70</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>750</v>
+      </c>
+      <c r="M5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11377</v>
+      </c>
+      <c r="B6">
+        <v>11377</v>
+      </c>
+      <c r="C6">
+        <v>11377</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5">
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <v>18</v>
+      </c>
+      <c r="L6">
+        <v>360</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11377</v>
+      </c>
+      <c r="B7">
+        <v>11377</v>
+      </c>
+      <c r="C7">
+        <v>11377</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7">
         <v>2</v>
       </c>
-      <c r="M5">
-        <v>59</v>
-      </c>
-      <c r="N5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="L7">
+        <v>55</v>
+      </c>
+      <c r="M7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" t="s">
         <v>22</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="X5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -4927,6 +4732,299 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A641F-CDF5-42AA-90C2-89A89CF0D81F}">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>2199</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
+      <c r="L3">
+        <v>324</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>59</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11377</v>
+      </c>
+      <c r="B5">
+        <v>11377</v>
+      </c>
+      <c r="C5">
+        <v>11377</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>59</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0702AE-AE2A-4040-B020-48654513E736}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -5075,7 +5173,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -5128,7 +5226,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -5181,223 +5279,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C9544C-A3E8-4087-8CA1-7B6068AB4469}">
-  <dimension ref="A1:Y3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="5" max="6" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2">
-        <v>59</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="V2" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <v>2199</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>36</v>
-      </c>
-      <c r="M3">
-        <v>259</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V3" t="s">
-        <v>27</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change in excel data file reader
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-vkaushal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB37286-A929-4187-8836-8F3B84317EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1CF67C-48BC-44D1-BD59-662F821E7A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" firstSheet="4" activeTab="4" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" firstSheet="7" activeTab="9" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="87">
   <si>
     <t>AgentCode</t>
   </si>
@@ -283,18 +283,6 @@
   </si>
   <si>
     <t>PET CONNECT</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00009</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00010</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00011</t>
-  </si>
-  <si>
-    <t>LTE001_ACC_00012</t>
   </si>
   <si>
     <t>LTE001_ACC_00015</t>
@@ -705,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15025949-10D9-4C1B-9506-C6E07A0B91EB}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,213 +809,172 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C9544C-A3E8-4087-8CA1-7B6068AB4469}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="5" max="6" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="L2">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>2199</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>36</v>
+      </c>
+      <c r="L3">
+        <v>259</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2">
-        <v>59</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="V2" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="P3" t="s">
         <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <v>2199</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>36</v>
-      </c>
-      <c r="M3">
-        <v>259</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V3" t="s">
-        <v>27</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1037,260 +984,199 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588B3A75-C7DB-40C6-BCDF-882DAD4C0277}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>775</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>2199</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>360</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>13</v>
-      </c>
-      <c r="M2">
-        <v>775</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <v>2199</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>8</v>
-      </c>
-      <c r="M3">
-        <v>360</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>11377</v>
-      </c>
-      <c r="C4">
-        <v>11377</v>
-      </c>
-      <c r="D4">
-        <v>11377</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
       <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
         <v>59</v>
       </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
       <c r="N4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1300,27 +1186,26 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F85EB7-D4FE-4731-A89B-6B56A2672E3B}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection sqref="A1:Y1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1328,232 +1213,172 @@
         <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="D2">
+      <c r="C2">
         <v>10763</v>
       </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
-        <v>18</v>
+      <c r="K2">
+        <v>13</v>
       </c>
       <c r="L2">
-        <v>13</v>
-      </c>
-      <c r="M2">
         <v>775</v>
       </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
       <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <v>10763</v>
       </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="H3">
         <v>2199</v>
       </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
       <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" t="s">
-        <v>18</v>
+      <c r="K3">
+        <v>8</v>
       </c>
       <c r="L3">
-        <v>8</v>
-      </c>
-      <c r="M3">
         <v>360</v>
       </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
       <c r="N3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>10763</v>
       </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" t="s">
-        <v>18</v>
+      <c r="K4">
+        <v>2</v>
       </c>
       <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
         <v>59</v>
       </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
       <c r="N4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1729,7 +1554,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1797,7 +1622,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1865,7 +1690,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2022,7 +1847,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2137,7 +1962,7 @@
         <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -2179,7 +2004,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2190,7 +2015,7 @@
         <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
@@ -2232,7 +2057,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2389,7 +2214,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2550,7 +2375,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2606,7 +2431,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2763,7 +2588,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2920,7 +2745,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2973,7 +2798,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -3026,7 +2851,7 @@
         <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3401,7 +3226,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -3457,7 +3282,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -4125,9 +3950,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA38A178-4DE0-471C-BD3C-CC9822D93DCD}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -4339,7 +4164,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -4356,7 +4181,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -4735,8 +4560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A641F-CDF5-42AA-90C2-89A89CF0D81F}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4844,10 +4669,10 @@
         <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O2" t="s">
         <v>22</v>
@@ -4897,10 +4722,10 @@
         <v>324</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O3" t="s">
         <v>22</v>
@@ -4950,10 +4775,10 @@
         <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O4" t="s">
         <v>22</v>
@@ -5003,10 +4828,10 @@
         <v>59</v>
       </c>
       <c r="M5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O5" t="s">
         <v>22</v>
@@ -5026,260 +4851,199 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0702AE-AE2A-4040-B020-48654513E736}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>775</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L3">
+        <v>200</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2">
-        <v>11377</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>13</v>
-      </c>
-      <c r="M2">
-        <v>775</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="L4">
+        <v>840</v>
+      </c>
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11377</v>
-      </c>
-      <c r="C3">
-        <v>11377</v>
-      </c>
-      <c r="D3">
-        <v>11377</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3">
-        <v>6</v>
-      </c>
-      <c r="M3">
-        <v>200</v>
-      </c>
-      <c r="N3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>11377</v>
-      </c>
-      <c r="C4">
-        <v>11377</v>
-      </c>
-      <c r="D4">
-        <v>11377</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4">
-        <v>8</v>
-      </c>
-      <c r="M4">
-        <v>840</v>
-      </c>
       <c r="N4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated role and driver
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-vkaushal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86F0D50-D4CA-4456-A209-7B0FDACF835B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB2EC66-DF29-434B-80C6-3CE342D6CB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" firstSheet="15" activeTab="18" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" firstSheet="5" activeTab="5" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -1666,8 +1666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E9B1A2-8828-4F98-87B5-7CAF91123FE0}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,7 +1869,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,10 +1939,10 @@
         <v>10763</v>
       </c>
       <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
       </c>
       <c r="F2" t="s">
         <v>58</v>
@@ -1966,10 +1966,10 @@
         <v>87</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1983,7 +1983,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,8 +2254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6658BEBD-BE9E-40E4-8B04-B10FCCEDE4E2}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2332,7 +2332,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -2356,10 +2356,10 @@
         <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O2" t="s">
         <v>50</v>
@@ -4134,8 +4134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D71B933-D35A-4F10-8F8D-DB21B7A241A8}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4168,7 +4168,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Change in excel of LTE
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-vkaushal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2025\Xunit Sprint 7\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB2EC66-DF29-434B-80C6-3CE342D6CB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C062531-F689-4CF9-82DC-96D9816F5E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" firstSheet="5" activeTab="5" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19190" windowHeight="10190" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="80">
   <si>
     <t>AgentCode</t>
   </si>
@@ -672,23 +672,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15025949-10D9-4C1B-9506-C6E07A0B91EB}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -779,6 +779,194 @@
         <v>18</v>
       </c>
       <c r="O2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>750</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>11377</v>
+      </c>
+      <c r="B5">
+        <v>11377</v>
+      </c>
+      <c r="C5">
+        <v>11377</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>600</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>11377</v>
+      </c>
+      <c r="B6">
+        <v>11377</v>
+      </c>
+      <c r="C6">
+        <v>11377</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -796,19 +984,19 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="4" max="5" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="4" max="5" width="12.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +1046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -908,7 +1096,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -971,20 +1159,20 @@
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" customWidth="1"/>
+    <col min="13" max="13" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -1072,7 +1260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -1116,7 +1304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -1173,20 +1361,20 @@
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
+    <col min="13" max="13" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1230,7 +1418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1274,7 +1462,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1318,7 +1506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1376,9 +1564,9 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1422,7 +1610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -1466,7 +1654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -1523,9 +1711,9 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10763</v>
       </c>
@@ -1613,7 +1801,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -1670,19 +1858,19 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="4" max="5" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="4" max="5" width="14.1796875" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" customWidth="1"/>
+    <col min="8" max="8" width="19.26953125" customWidth="1"/>
+    <col min="9" max="9" width="18.26953125" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -1770,7 +1958,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -1814,7 +2002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -1872,19 +2060,19 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +2116,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1986,20 +2174,20 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" customWidth="1"/>
+    <col min="13" max="13" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2043,7 +2231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2087,7 +2275,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2144,20 +2332,20 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2201,7 +2389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2258,20 +2446,20 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2318,7 +2506,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -2365,7 +2553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -2425,20 +2613,20 @@
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2485,7 +2673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2532,7 +2720,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2579,7 +2767,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2639,21 +2827,21 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" customWidth="1"/>
+    <col min="9" max="9" width="20.81640625" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="14" max="14" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2730,7 +2918,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2796,21 +2984,21 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" customWidth="1"/>
+    <col min="10" max="10" width="16.54296875" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2887,7 +3075,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2940,7 +3128,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2993,7 +3181,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -3059,22 +3247,22 @@
       <selection activeCell="A2" sqref="A2:Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="18.7265625" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" customWidth="1"/>
+    <col min="15" max="15" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3151,7 +3339,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -3207,7 +3395,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -3276,25 +3464,25 @@
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="14.54296875" customWidth="1"/>
+    <col min="16" max="16" width="28.453125" customWidth="1"/>
     <col min="17" max="17" width="17" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.1796875" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" customWidth="1"/>
+    <col min="20" max="20" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3356,7 +3544,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -3418,7 +3606,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -3480,7 +3668,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -3542,7 +3730,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>11377</v>
       </c>
@@ -3604,7 +3792,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>11377</v>
       </c>
@@ -3666,40 +3854,40 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R8" s="2"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R14" s="2"/>
     </row>
-    <row r="17" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R17" s="2"/>
     </row>
-    <row r="20" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R20" s="2"/>
     </row>
-    <row r="22" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R25" s="2"/>
     </row>
   </sheetData>
@@ -3716,17 +3904,17 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3773,7 +3961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -3820,7 +4008,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -3867,7 +4055,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -3914,10 +4102,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="H5" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="H7" s="1"/>
     </row>
   </sheetData>
@@ -3934,21 +4122,21 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3992,7 +4180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4036,7 +4224,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -4080,7 +4268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -4134,13 +4322,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D71B933-D35A-4F10-8F8D-DB21B7A241A8}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -4157,7 +4345,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -4187,20 +4375,20 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4247,7 +4435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4294,7 +4482,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -4341,7 +4529,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -4388,7 +4576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>11377</v>
       </c>
@@ -4435,7 +4623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>11377</v>
       </c>
@@ -4482,7 +4670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>11377</v>
       </c>
@@ -4542,21 +4730,21 @@
       <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" customWidth="1"/>
+    <col min="15" max="15" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4609,7 +4797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4662,7 +4850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -4715,7 +4903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -4768,7 +4956,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>11377</v>
       </c>
@@ -4835,20 +5023,20 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4892,7 +5080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4936,7 +5124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -4980,7 +5168,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>

</xml_diff>

<commit_message>
Change in LTE001 excel
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2025\Xunit Sprint 7\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C062531-F689-4CF9-82DC-96D9816F5E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676AB2C5-5BE1-471E-BF0F-9D1D8A9A73F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19190" windowHeight="10190" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -675,7 +675,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -796,7 +796,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Adding OPR293 test scenario
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-vkaushal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2025\Xunit Sprint 7\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB2EC66-DF29-434B-80C6-3CE342D6CB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C062531-F689-4CF9-82DC-96D9816F5E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" firstSheet="5" activeTab="5" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19190" windowHeight="10190" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="80">
   <si>
     <t>AgentCode</t>
   </si>
@@ -672,23 +672,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15025949-10D9-4C1B-9506-C6E07A0B91EB}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -779,6 +779,194 @@
         <v>18</v>
       </c>
       <c r="O2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>750</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>11377</v>
+      </c>
+      <c r="B4">
+        <v>11377</v>
+      </c>
+      <c r="C4">
+        <v>11377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>11377</v>
+      </c>
+      <c r="B5">
+        <v>11377</v>
+      </c>
+      <c r="C5">
+        <v>11377</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>600</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>11377</v>
+      </c>
+      <c r="B6">
+        <v>11377</v>
+      </c>
+      <c r="C6">
+        <v>11377</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -796,19 +984,19 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="4" max="5" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="4" max="5" width="12.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +1046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -908,7 +1096,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -971,20 +1159,20 @@
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" customWidth="1"/>
+    <col min="13" max="13" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -1072,7 +1260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -1116,7 +1304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -1173,20 +1361,20 @@
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
+    <col min="13" max="13" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1230,7 +1418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1274,7 +1462,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1318,7 +1506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1376,9 +1564,9 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1422,7 +1610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -1466,7 +1654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -1523,9 +1711,9 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10763</v>
       </c>
@@ -1613,7 +1801,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -1670,19 +1858,19 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="4" max="5" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="4" max="5" width="14.1796875" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" customWidth="1"/>
+    <col min="8" max="8" width="19.26953125" customWidth="1"/>
+    <col min="9" max="9" width="18.26953125" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -1770,7 +1958,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -1814,7 +2002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -1872,19 +2060,19 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +2116,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1986,20 +2174,20 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" customWidth="1"/>
+    <col min="13" max="13" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2043,7 +2231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2087,7 +2275,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2144,20 +2332,20 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2201,7 +2389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2258,20 +2446,20 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2318,7 +2506,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -2365,7 +2553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -2425,20 +2613,20 @@
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2485,7 +2673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2532,7 +2720,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2579,7 +2767,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2639,21 +2827,21 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" customWidth="1"/>
+    <col min="9" max="9" width="20.81640625" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="14" max="14" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2730,7 +2918,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2796,21 +2984,21 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" customWidth="1"/>
+    <col min="10" max="10" width="16.54296875" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2887,7 +3075,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2940,7 +3128,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2993,7 +3181,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -3059,22 +3247,22 @@
       <selection activeCell="A2" sqref="A2:Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="18.7265625" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" customWidth="1"/>
+    <col min="15" max="15" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3151,7 +3339,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -3207,7 +3395,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -3276,25 +3464,25 @@
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="14.54296875" customWidth="1"/>
+    <col min="16" max="16" width="28.453125" customWidth="1"/>
     <col min="17" max="17" width="17" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.1796875" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" customWidth="1"/>
+    <col min="20" max="20" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3356,7 +3544,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -3418,7 +3606,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -3480,7 +3668,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -3542,7 +3730,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>11377</v>
       </c>
@@ -3604,7 +3792,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>11377</v>
       </c>
@@ -3666,40 +3854,40 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R8" s="2"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R14" s="2"/>
     </row>
-    <row r="17" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R17" s="2"/>
     </row>
-    <row r="20" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R20" s="2"/>
     </row>
-    <row r="22" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R25" s="2"/>
     </row>
   </sheetData>
@@ -3716,17 +3904,17 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3773,7 +3961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -3820,7 +4008,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -3867,7 +4055,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -3914,10 +4102,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="H5" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="H7" s="1"/>
     </row>
   </sheetData>
@@ -3934,21 +4122,21 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3992,7 +4180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4036,7 +4224,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -4080,7 +4268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -4134,13 +4322,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D71B933-D35A-4F10-8F8D-DB21B7A241A8}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -4157,7 +4345,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -4187,20 +4375,20 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4247,7 +4435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4294,7 +4482,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -4341,7 +4529,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -4388,7 +4576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>11377</v>
       </c>
@@ -4435,7 +4623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>11377</v>
       </c>
@@ -4482,7 +4670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>11377</v>
       </c>
@@ -4542,21 +4730,21 @@
       <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" customWidth="1"/>
+    <col min="15" max="15" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4609,7 +4797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4662,7 +4850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -4715,7 +4903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -4768,7 +4956,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>11377</v>
       </c>
@@ -4835,20 +5023,20 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4892,7 +5080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4936,7 +5124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -4980,7 +5168,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>

</xml_diff>

<commit_message>
Adding updated test data
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-ssaha1\Desktop\ICargo KT\Test data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8813C214-93A2-4C6F-8E96-FC5017B8F460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339055CF-4709-4999-9FEA-B905D3605651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="11" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -6399,7 +6399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F85EB7-D4FE-4731-A89B-6B56A2672E3B}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -8414,8 +8414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02740B3-88E5-4DDF-8354-11DFF949E13D}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8707,10 +8707,10 @@
         <v>144</v>
       </c>
       <c r="M6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O6" t="s">
         <v>22</v>
@@ -8754,10 +8754,10 @@
         <v>100</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O7" t="s">
         <v>22</v>
@@ -8801,10 +8801,10 @@
         <v>66</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O8" t="s">
         <v>22</v>
@@ -8848,10 +8848,10 @@
         <v>100</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O9" t="s">
         <v>22</v>
@@ -9130,10 +9130,10 @@
         <v>60</v>
       </c>
       <c r="M15" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O15" t="s">
         <v>22</v>
@@ -9177,10 +9177,10 @@
         <v>70</v>
       </c>
       <c r="M16" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O16" t="s">
         <v>22</v>
@@ -9224,10 +9224,10 @@
         <v>80</v>
       </c>
       <c r="M17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O17" t="s">
         <v>22</v>
@@ -9271,10 +9271,10 @@
         <v>90</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O18" t="s">
         <v>22</v>
@@ -9412,10 +9412,10 @@
         <v>160</v>
       </c>
       <c r="M21" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O21" t="s">
         <v>22</v>
@@ -10067,8 +10067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55333C5B-4CB8-438D-AA05-F854870A7A77}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10191,10 +10191,10 @@
         <v>175</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O2" t="s">
         <v>22</v>
@@ -10253,10 +10253,10 @@
         <v>360</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O3" t="s">
         <v>22</v>
@@ -10315,10 +10315,10 @@
         <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O4" t="s">
         <v>22</v>
@@ -10501,10 +10501,10 @@
         <v>100</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O7" t="s">
         <v>22</v>
@@ -10563,10 +10563,10 @@
         <v>66</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O8" t="s">
         <v>22</v>
@@ -10873,10 +10873,10 @@
         <v>40</v>
       </c>
       <c r="M13" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O13" t="s">
         <v>22</v>
@@ -10935,10 +10935,10 @@
         <v>50</v>
       </c>
       <c r="M14" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O14" t="s">
         <v>22</v>
@@ -11121,10 +11121,10 @@
         <v>80</v>
       </c>
       <c r="M17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O17" t="s">
         <v>22</v>
@@ -11183,10 +11183,10 @@
         <v>90</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O18" t="s">
         <v>22</v>
@@ -11369,10 +11369,10 @@
         <v>160</v>
       </c>
       <c r="M21" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O21" t="s">
         <v>22</v>
@@ -11431,10 +11431,10 @@
         <v>175</v>
       </c>
       <c r="M22" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O22" t="s">
         <v>22</v>
@@ -11493,10 +11493,10 @@
         <v>360</v>
       </c>
       <c r="M23" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O23" t="s">
         <v>22</v>
@@ -11555,10 +11555,10 @@
         <v>59</v>
       </c>
       <c r="M24" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O24" t="s">
         <v>22</v>
@@ -11741,10 +11741,10 @@
         <v>100</v>
       </c>
       <c r="M27" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O27" t="s">
         <v>22</v>
@@ -11803,10 +11803,10 @@
         <v>66</v>
       </c>
       <c r="M28" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O28" t="s">
         <v>22</v>
@@ -12113,10 +12113,10 @@
         <v>40</v>
       </c>
       <c r="M33" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N33" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O33" t="s">
         <v>22</v>
@@ -12175,10 +12175,10 @@
         <v>50</v>
       </c>
       <c r="M34" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N34" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O34" t="s">
         <v>22</v>
@@ -12361,10 +12361,10 @@
         <v>80</v>
       </c>
       <c r="M37" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N37" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O37" t="s">
         <v>22</v>
@@ -12423,10 +12423,10 @@
         <v>90</v>
       </c>
       <c r="M38" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O38" t="s">
         <v>22</v>
@@ -12609,10 +12609,10 @@
         <v>160</v>
       </c>
       <c r="M41" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N41" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O41" t="s">
         <v>22</v>
@@ -12671,10 +12671,10 @@
         <v>175</v>
       </c>
       <c r="M42" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O42" t="s">
         <v>22</v>
@@ -12733,10 +12733,10 @@
         <v>360</v>
       </c>
       <c r="M43" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N43" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O43" t="s">
         <v>22</v>
@@ -12795,10 +12795,10 @@
         <v>59</v>
       </c>
       <c r="M44" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N44" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O44" t="s">
         <v>22</v>
@@ -12981,10 +12981,10 @@
         <v>100</v>
       </c>
       <c r="M47" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N47" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O47" t="s">
         <v>22</v>
@@ -13043,10 +13043,10 @@
         <v>66</v>
       </c>
       <c r="M48" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N48" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O48" t="s">
         <v>22</v>
@@ -13263,8 +13263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE920C76-3A37-4057-8B20-893482492082}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13365,10 +13365,10 @@
         <v>177</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O2" t="s">
         <v>22</v>
@@ -13412,10 +13412,10 @@
         <v>128</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O3" t="s">
         <v>22</v>
@@ -13459,10 +13459,10 @@
         <v>55</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O4" t="s">
         <v>22</v>
@@ -13553,10 +13553,10 @@
         <v>124</v>
       </c>
       <c r="M6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O6" t="s">
         <v>22</v>
@@ -13600,10 +13600,10 @@
         <v>100</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O7" t="s">
         <v>22</v>
@@ -13647,10 +13647,10 @@
         <v>66</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O8" t="s">
         <v>22</v>
@@ -13694,10 +13694,10 @@
         <v>100</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O9" t="s">
         <v>22</v>
@@ -13976,10 +13976,10 @@
         <v>60</v>
       </c>
       <c r="M15" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O15" t="s">
         <v>22</v>
@@ -14023,10 +14023,10 @@
         <v>70</v>
       </c>
       <c r="M16" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O16" t="s">
         <v>22</v>
@@ -14070,10 +14070,10 @@
         <v>80</v>
       </c>
       <c r="M17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O17" t="s">
         <v>22</v>
@@ -14117,10 +14117,10 @@
         <v>90</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O18" t="s">
         <v>22</v>
@@ -14305,10 +14305,10 @@
         <v>177</v>
       </c>
       <c r="M22" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O22" t="s">
         <v>22</v>
@@ -14352,10 +14352,10 @@
         <v>128</v>
       </c>
       <c r="M23" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O23" t="s">
         <v>22</v>
@@ -14399,10 +14399,10 @@
         <v>55</v>
       </c>
       <c r="M24" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O24" t="s">
         <v>22</v>
@@ -14493,10 +14493,10 @@
         <v>124</v>
       </c>
       <c r="M26" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O26" t="s">
         <v>22</v>
@@ -14540,10 +14540,10 @@
         <v>100</v>
       </c>
       <c r="M27" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O27" t="s">
         <v>22</v>
@@ -14587,10 +14587,10 @@
         <v>66</v>
       </c>
       <c r="M28" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O28" t="s">
         <v>22</v>
@@ -14634,10 +14634,10 @@
         <v>100</v>
       </c>
       <c r="M29" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O29" t="s">
         <v>22</v>
@@ -14916,10 +14916,10 @@
         <v>60</v>
       </c>
       <c r="M35" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O35" t="s">
         <v>22</v>
@@ -14963,10 +14963,10 @@
         <v>70</v>
       </c>
       <c r="M36" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N36" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O36" t="s">
         <v>22</v>
@@ -15010,10 +15010,10 @@
         <v>80</v>
       </c>
       <c r="M37" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N37" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O37" t="s">
         <v>22</v>
@@ -15057,10 +15057,10 @@
         <v>90</v>
       </c>
       <c r="M38" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O38" t="s">
         <v>22</v>
@@ -15245,10 +15245,10 @@
         <v>177</v>
       </c>
       <c r="M42" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O42" t="s">
         <v>22</v>
@@ -15292,10 +15292,10 @@
         <v>128</v>
       </c>
       <c r="M43" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N43" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O43" t="s">
         <v>22</v>
@@ -15339,10 +15339,10 @@
         <v>55</v>
       </c>
       <c r="M44" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N44" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O44" t="s">
         <v>22</v>
@@ -15433,10 +15433,10 @@
         <v>124</v>
       </c>
       <c r="M46" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N46" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O46" t="s">
         <v>22</v>
@@ -15480,10 +15480,10 @@
         <v>100</v>
       </c>
       <c r="M47" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N47" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O47" t="s">
         <v>22</v>
@@ -15527,10 +15527,10 @@
         <v>66</v>
       </c>
       <c r="M48" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N48" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O48" t="s">
         <v>22</v>
@@ -15574,10 +15574,10 @@
         <v>100</v>
       </c>
       <c r="M49" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N49" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O49" t="s">
         <v>22</v>
@@ -15687,8 +15687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA38A178-4DE0-471C-BD3C-CC9822D93DCD}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView topLeftCell="H40" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15705,6 +15705,7 @@
     <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="15.1796875" customWidth="1"/>
+    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.7265625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15969,10 +15970,10 @@
         <v>124</v>
       </c>
       <c r="M6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O6" t="s">
         <v>22</v>
@@ -16016,10 +16017,10 @@
         <v>100</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O7" t="s">
         <v>22</v>
@@ -16063,10 +16064,10 @@
         <v>66</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O8" t="s">
         <v>22</v>
@@ -16110,10 +16111,10 @@
         <v>100</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O9" t="s">
         <v>22</v>
@@ -16392,10 +16393,10 @@
         <v>60</v>
       </c>
       <c r="M15" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O15" t="s">
         <v>22</v>
@@ -16439,10 +16440,10 @@
         <v>70</v>
       </c>
       <c r="M16" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O16" t="s">
         <v>22</v>
@@ -16486,10 +16487,10 @@
         <v>80</v>
       </c>
       <c r="M17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O17" t="s">
         <v>22</v>
@@ -16533,10 +16534,10 @@
         <v>90</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O18" t="s">
         <v>22</v>
@@ -16897,10 +16898,10 @@
         <v>124</v>
       </c>
       <c r="M26" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
@@ -16941,10 +16942,10 @@
         <v>100</v>
       </c>
       <c r="M27" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
@@ -16985,10 +16986,10 @@
         <v>66</v>
       </c>
       <c r="M28" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
@@ -17029,10 +17030,10 @@
         <v>100</v>
       </c>
       <c r="M29" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
@@ -17293,10 +17294,10 @@
         <v>60</v>
       </c>
       <c r="M35" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
@@ -17337,10 +17338,10 @@
         <v>70</v>
       </c>
       <c r="M36" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N36" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
@@ -17381,10 +17382,10 @@
         <v>80</v>
       </c>
       <c r="M37" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N37" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
@@ -17425,10 +17426,10 @@
         <v>90</v>
       </c>
       <c r="M38" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
@@ -17601,10 +17602,10 @@
         <v>100</v>
       </c>
       <c r="M42" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
@@ -17645,10 +17646,10 @@
         <v>66</v>
       </c>
       <c r="M43" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N43" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
@@ -17689,10 +17690,10 @@
         <v>100</v>
       </c>
       <c r="M44" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N44" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
@@ -17953,10 +17954,10 @@
         <v>60</v>
       </c>
       <c r="M50" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N50" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
@@ -17997,10 +17998,10 @@
         <v>70</v>
       </c>
       <c r="M51" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N51" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -18060,8 +18061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1051281-76C6-44DD-9FC2-1F77E64E8898}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18492,10 +18493,10 @@
         <v>124</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O9" t="s">
         <v>22</v>
@@ -18539,10 +18540,10 @@
         <v>100</v>
       </c>
       <c r="M10" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O10" t="s">
         <v>22</v>
@@ -18586,10 +18587,10 @@
         <v>66</v>
       </c>
       <c r="M11" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O11" t="s">
         <v>22</v>
@@ -18633,10 +18634,10 @@
         <v>100</v>
       </c>
       <c r="M12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O12" t="s">
         <v>22</v>
@@ -18915,10 +18916,10 @@
         <v>60</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O18" t="s">
         <v>22</v>
@@ -18962,10 +18963,10 @@
         <v>70</v>
       </c>
       <c r="M19" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O19" t="s">
         <v>22</v>
@@ -19009,10 +19010,10 @@
         <v>80</v>
       </c>
       <c r="M20" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O20" t="s">
         <v>22</v>
@@ -19056,10 +19057,10 @@
         <v>90</v>
       </c>
       <c r="M21" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O21" t="s">
         <v>22</v>
@@ -19432,10 +19433,10 @@
         <v>124</v>
       </c>
       <c r="M29" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O29" t="s">
         <v>22</v>
@@ -19479,10 +19480,10 @@
         <v>100</v>
       </c>
       <c r="M30" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O30" t="s">
         <v>22</v>
@@ -19526,10 +19527,10 @@
         <v>66</v>
       </c>
       <c r="M31" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N31" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O31" t="s">
         <v>22</v>
@@ -19573,10 +19574,10 @@
         <v>100</v>
       </c>
       <c r="M32" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N32" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O32" t="s">
         <v>22</v>
@@ -19855,10 +19856,10 @@
         <v>60</v>
       </c>
       <c r="M38" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O38" t="s">
         <v>22</v>
@@ -19902,10 +19903,10 @@
         <v>70</v>
       </c>
       <c r="M39" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N39" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O39" t="s">
         <v>22</v>
@@ -19949,10 +19950,10 @@
         <v>80</v>
       </c>
       <c r="M40" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N40" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O40" t="s">
         <v>22</v>
@@ -19996,10 +19997,10 @@
         <v>90</v>
       </c>
       <c r="M41" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N41" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O41" t="s">
         <v>22</v>
@@ -20043,10 +20044,10 @@
         <v>100</v>
       </c>
       <c r="M42" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O42" t="s">
         <v>22</v>
@@ -20090,10 +20091,10 @@
         <v>66</v>
       </c>
       <c r="M43" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N43" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O43" t="s">
         <v>22</v>
@@ -20137,10 +20138,10 @@
         <v>100</v>
       </c>
       <c r="M44" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N44" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O44" t="s">
         <v>22</v>
@@ -20419,10 +20420,10 @@
         <v>60</v>
       </c>
       <c r="M50" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N50" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O50" t="s">
         <v>22</v>
@@ -20466,10 +20467,10 @@
         <v>70</v>
       </c>
       <c r="M51" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N51" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O51" t="s">
         <v>22</v>
@@ -20485,8 +20486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A641F-CDF5-42AA-90C2-89A89CF0D81F}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView topLeftCell="E40" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView topLeftCell="E37" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20845,10 +20846,10 @@
         <v>124</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O7" t="s">
         <v>22</v>
@@ -20895,10 +20896,10 @@
         <v>100</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O8" t="s">
         <v>22</v>
@@ -20945,10 +20946,10 @@
         <v>66</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O9" t="s">
         <v>22</v>
@@ -20995,10 +20996,10 @@
         <v>100</v>
       </c>
       <c r="M10" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O10" t="s">
         <v>22</v>
@@ -21295,10 +21296,10 @@
         <v>60</v>
       </c>
       <c r="M16" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O16" t="s">
         <v>22</v>
@@ -21345,10 +21346,10 @@
         <v>70</v>
       </c>
       <c r="M17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O17" t="s">
         <v>22</v>
@@ -21395,10 +21396,10 @@
         <v>80</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O18" t="s">
         <v>22</v>
@@ -21445,10 +21446,10 @@
         <v>90</v>
       </c>
       <c r="M19" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O19" t="s">
         <v>22</v>
@@ -21845,10 +21846,10 @@
         <v>124</v>
       </c>
       <c r="M27" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O27" t="s">
         <v>22</v>
@@ -21895,10 +21896,10 @@
         <v>100</v>
       </c>
       <c r="M28" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O28" t="s">
         <v>22</v>
@@ -21945,10 +21946,10 @@
         <v>66</v>
       </c>
       <c r="M29" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O29" t="s">
         <v>22</v>
@@ -21995,10 +21996,10 @@
         <v>100</v>
       </c>
       <c r="M30" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O30" t="s">
         <v>22</v>
@@ -22295,10 +22296,10 @@
         <v>60</v>
       </c>
       <c r="M36" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N36" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O36" t="s">
         <v>22</v>
@@ -22345,10 +22346,10 @@
         <v>70</v>
       </c>
       <c r="M37" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N37" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O37" t="s">
         <v>22</v>
@@ -22395,10 +22396,10 @@
         <v>80</v>
       </c>
       <c r="M38" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O38" t="s">
         <v>22</v>
@@ -22445,10 +22446,10 @@
         <v>90</v>
       </c>
       <c r="M39" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N39" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O39" t="s">
         <v>22</v>
@@ -22845,10 +22846,10 @@
         <v>124</v>
       </c>
       <c r="M47" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N47" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O47" t="s">
         <v>22</v>
@@ -22895,10 +22896,10 @@
         <v>100</v>
       </c>
       <c r="M48" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N48" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O48" t="s">
         <v>22</v>
@@ -22945,10 +22946,10 @@
         <v>66</v>
       </c>
       <c r="M49" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N49" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O49" t="s">
         <v>22</v>
@@ -22995,10 +22996,10 @@
         <v>100</v>
       </c>
       <c r="M50" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N50" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O50" t="s">
         <v>22</v>
@@ -23067,8 +23068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0702AE-AE2A-4040-B020-48654513E736}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N49"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Adding changed data of LTE001
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-ssaha1\Desktop\ICargo KT\Test data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E74F27F-4DC4-4D5D-A513-B82FF2E48581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E874F210-463F-4C88-B9CB-0B6264073477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="7" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4899" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4882" uniqueCount="83">
   <si>
     <t>AgentCode</t>
   </si>
@@ -15685,10 +15685,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA38A178-4DE0-471C-BD3C-CC9822D93DCD}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15706,10 +15706,10 @@
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="15.1796875" customWidth="1"/>
     <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7265625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="5.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15753,7 +15753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -15797,7 +15797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -15841,7 +15841,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -15885,7 +15885,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>11377</v>
       </c>
@@ -15928,11 +15928,8 @@
       <c r="N5" t="s">
         <v>21</v>
       </c>
-      <c r="O5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>11377</v>
       </c>
@@ -15975,11 +15972,8 @@
       <c r="N6" t="s">
         <v>21</v>
       </c>
-      <c r="O6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>11377</v>
       </c>
@@ -16022,11 +16016,8 @@
       <c r="N7" t="s">
         <v>21</v>
       </c>
-      <c r="O7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>11377</v>
       </c>
@@ -16069,11 +16060,8 @@
       <c r="N8" t="s">
         <v>21</v>
       </c>
-      <c r="O8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>11377</v>
       </c>
@@ -16116,11 +16104,8 @@
       <c r="N9" t="s">
         <v>21</v>
       </c>
-      <c r="O9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>11377</v>
       </c>
@@ -16163,11 +16148,8 @@
       <c r="N10" t="s">
         <v>21</v>
       </c>
-      <c r="O10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>11377</v>
       </c>
@@ -16210,11 +16192,8 @@
       <c r="N11" t="s">
         <v>21</v>
       </c>
-      <c r="O11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11377</v>
       </c>
@@ -16257,11 +16236,8 @@
       <c r="N12" t="s">
         <v>21</v>
       </c>
-      <c r="O12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11377</v>
       </c>
@@ -16304,11 +16280,8 @@
       <c r="N13" t="s">
         <v>21</v>
       </c>
-      <c r="O13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>11377</v>
       </c>
@@ -16351,11 +16324,8 @@
       <c r="N14" t="s">
         <v>21</v>
       </c>
-      <c r="O14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>11377</v>
       </c>
@@ -16398,11 +16368,8 @@
       <c r="N15" t="s">
         <v>21</v>
       </c>
-      <c r="O15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>11377</v>
       </c>
@@ -16445,11 +16412,8 @@
       <c r="N16" t="s">
         <v>21</v>
       </c>
-      <c r="O16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>11377</v>
       </c>
@@ -16492,11 +16456,8 @@
       <c r="N17" t="s">
         <v>21</v>
       </c>
-      <c r="O17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>11377</v>
       </c>
@@ -16539,11 +16500,8 @@
       <c r="N18" t="s">
         <v>21</v>
       </c>
-      <c r="O18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>11377</v>
       </c>
@@ -16586,11 +16544,8 @@
       <c r="N19" t="s">
         <v>21</v>
       </c>
-      <c r="O19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>11377</v>
       </c>
@@ -16633,11 +16588,8 @@
       <c r="N20" t="s">
         <v>21</v>
       </c>
-      <c r="O20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>11377</v>
       </c>
@@ -16680,11 +16632,8 @@
       <c r="N21" t="s">
         <v>21</v>
       </c>
-      <c r="O21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>11377</v>
       </c>
@@ -16728,7 +16677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>11377</v>
       </c>
@@ -16772,7 +16721,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>11377</v>
       </c>
@@ -16816,7 +16765,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>11377</v>
       </c>
@@ -16860,7 +16809,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>11377</v>
       </c>
@@ -16904,7 +16853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>11377</v>
       </c>
@@ -16948,7 +16897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>11377</v>
       </c>
@@ -16992,7 +16941,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>11377</v>
       </c>
@@ -17036,7 +16985,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>11377</v>
       </c>
@@ -17080,7 +17029,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>11377</v>
       </c>
@@ -17124,7 +17073,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>11377</v>
       </c>
@@ -18062,7 +18011,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A51"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18254,7 +18203,7 @@
         <v>18</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L4">
         <v>55</v>
@@ -18395,7 +18344,7 @@
         <v>18</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L7">
         <v>55</v>
@@ -18442,7 +18391,7 @@
         <v>18</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L8">
         <v>10</v>
@@ -18630,7 +18579,7 @@
         <v>18</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L12">
         <v>100</v>
@@ -18724,7 +18673,7 @@
         <v>18</v>
       </c>
       <c r="K14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L14">
         <v>20</v>
@@ -18771,7 +18720,7 @@
         <v>18</v>
       </c>
       <c r="K15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L15">
         <v>30</v>
@@ -19078,8 +19027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A641F-CDF5-42AA-90C2-89A89CF0D81F}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19382,7 +19331,7 @@
         <v>18</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L6">
         <v>10</v>
@@ -19482,7 +19431,7 @@
         <v>18</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L8">
         <v>100</v>
@@ -19582,7 +19531,7 @@
         <v>18</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L10">
         <v>100</v>
@@ -20382,7 +20331,7 @@
         <v>18</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L26">
         <v>10</v>
@@ -20482,7 +20431,7 @@
         <v>18</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L28">
         <v>100</v>
@@ -20582,7 +20531,7 @@
         <v>18</v>
       </c>
       <c r="K30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L30">
         <v>100</v>
@@ -21382,7 +21331,7 @@
         <v>18</v>
       </c>
       <c r="K46">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L46">
         <v>10</v>
@@ -21482,7 +21431,7 @@
         <v>18</v>
       </c>
       <c r="K48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L48">
         <v>100</v>
@@ -21582,7 +21531,7 @@
         <v>18</v>
       </c>
       <c r="K50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L50">
         <v>100</v>

</xml_diff>

<commit_message>
Change in home page
</commit_message>
<xml_diff>
--- a/TestData/LTE001_CreateShipment_TestData.xlsx
+++ b/TestData/LTE001_CreateShipment_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-ssaha1\Desktop\ICargo KT\Test data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB7A92B-61FA-4D59-BB65-E79EF0D2BEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28E7DA6-A685-49ED-B1D0-D1E8A7B18157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="7" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="9" xr2:uid="{065DB981-2341-4EA4-A395-B9D7BE870DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LTE001_ACC_00001" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4882" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4888" uniqueCount="83">
   <si>
     <t>AgentCode</t>
   </si>
@@ -1699,7 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C9544C-A3E8-4087-8CA1-7B6068AB4469}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
@@ -19027,8 +19027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7A641F-CDF5-42AA-90C2-89A89CF0D81F}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19171,8 +19171,8 @@
       <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="H3">
-        <v>2199</v>
+      <c r="H3" t="s">
+        <v>19</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -19266,7 +19266,7 @@
         <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -19310,10 +19310,10 @@
         <v>11377</v>
       </c>
       <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -19610,10 +19610,10 @@
         <v>11377</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
         <v>24</v>
@@ -19760,7 +19760,7 @@
         <v>11377</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
         <v>38</v>
@@ -19810,10 +19810,10 @@
         <v>11377</v>
       </c>
       <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
         <v>27</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
       </c>
       <c r="F16" t="s">
         <v>26</v>
@@ -19860,10 +19860,10 @@
         <v>11377</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
@@ -20171,8 +20171,8 @@
       <c r="G23" t="s">
         <v>18</v>
       </c>
-      <c r="H23">
-        <v>2199</v>
+      <c r="H23" t="s">
+        <v>19</v>
       </c>
       <c r="I23" t="s">
         <v>18</v>
@@ -20266,7 +20266,7 @@
         <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="G25" t="s">
         <v>18</v>
@@ -20310,10 +20310,10 @@
         <v>11377</v>
       </c>
       <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
         <v>38</v>
-      </c>
-      <c r="E26" t="s">
-        <v>16</v>
       </c>
       <c r="F26" t="s">
         <v>24</v>
@@ -20610,10 +20610,10 @@
         <v>11377</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="F32" t="s">
         <v>24</v>
@@ -20760,7 +20760,7 @@
         <v>11377</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="E35" t="s">
         <v>38</v>
@@ -20810,10 +20810,10 @@
         <v>11377</v>
       </c>
       <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
         <v>27</v>
-      </c>
-      <c r="E36" t="s">
-        <v>16</v>
       </c>
       <c r="F36" t="s">
         <v>26</v>
@@ -20860,10 +20860,10 @@
         <v>11377</v>
       </c>
       <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
         <v>38</v>
-      </c>
-      <c r="E37" t="s">
-        <v>50</v>
       </c>
       <c r="F37" t="s">
         <v>17</v>
@@ -21171,8 +21171,8 @@
       <c r="G43" t="s">
         <v>18</v>
       </c>
-      <c r="H43">
-        <v>2199</v>
+      <c r="H43" t="s">
+        <v>19</v>
       </c>
       <c r="I43" t="s">
         <v>18</v>
@@ -21266,7 +21266,7 @@
         <v>38</v>
       </c>
       <c r="F45" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="G45" t="s">
         <v>18</v>
@@ -21310,10 +21310,10 @@
         <v>11377</v>
       </c>
       <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" t="s">
         <v>38</v>
-      </c>
-      <c r="E46" t="s">
-        <v>16</v>
       </c>
       <c r="F46" t="s">
         <v>24</v>
@@ -21609,8 +21609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0702AE-AE2A-4040-B020-48654513E736}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21708,7 +21708,7 @@
         <v>13</v>
       </c>
       <c r="L2">
-        <v>775</v>
+        <v>77</v>
       </c>
       <c r="M2" t="s">
         <v>25</v>
@@ -21731,7 +21731,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -21752,7 +21752,7 @@
         <v>6</v>
       </c>
       <c r="L3">
-        <v>200</v>
+        <v>66</v>
       </c>
       <c r="M3" t="s">
         <v>25</v>
@@ -21775,10 +21775,10 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -21796,7 +21796,7 @@
         <v>8</v>
       </c>
       <c r="L4">
-        <v>840</v>
+        <v>88</v>
       </c>
       <c r="M4" t="s">
         <v>25</v>
@@ -21819,7 +21819,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
         <v>24</v>
@@ -21863,16 +21863,16 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="H6">
-        <v>2199</v>
+      <c r="H6" t="s">
+        <v>19</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -21884,7 +21884,7 @@
         <v>12</v>
       </c>
       <c r="L6">
-        <v>188</v>
+        <v>77</v>
       </c>
       <c r="M6" t="s">
         <v>25</v>
@@ -21907,7 +21907,7 @@
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -21951,10 +21951,10 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
@@ -21992,13 +21992,13 @@
         <v>11377</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
@@ -22042,7 +22042,7 @@
         <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G10" t="s">
         <v>18</v>
@@ -22060,7 +22060,7 @@
         <v>20</v>
       </c>
       <c r="L10">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="M10" t="s">
         <v>25</v>
@@ -22083,10 +22083,10 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
         <v>18</v>
@@ -22104,7 +22104,7 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="M11" t="s">
         <v>25</v>
@@ -22127,10 +22127,10 @@
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
@@ -22171,10 +22171,10 @@
         <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
@@ -22192,7 +22192,7 @@
         <v>1</v>
       </c>
       <c r="L13">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="M13" t="s">
         <v>25</v>
@@ -22215,7 +22215,7 @@
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -22236,7 +22236,7 @@
         <v>12</v>
       </c>
       <c r="L14">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="M14" t="s">
         <v>25</v>
@@ -22256,10 +22256,10 @@
         <v>11377</v>
       </c>
       <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
         <v>38</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
       </c>
       <c r="F15" t="s">
         <v>24</v>
@@ -22347,7 +22347,7 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
@@ -22388,10 +22388,10 @@
         <v>11377</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
@@ -22432,10 +22432,10 @@
         <v>11377</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
         <v>26</v>
@@ -22476,10 +22476,10 @@
         <v>11377</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
         <v>17</v>
@@ -22523,7 +22523,7 @@
         <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
@@ -22567,10 +22567,10 @@
         <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G22" t="s">
         <v>18</v>
@@ -22611,7 +22611,7 @@
         <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -22632,7 +22632,7 @@
         <v>10</v>
       </c>
       <c r="L23">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="M23" t="s">
         <v>25</v>
@@ -22655,10 +22655,10 @@
         <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G24" t="s">
         <v>18</v>
@@ -22676,7 +22676,7 @@
         <v>11</v>
       </c>
       <c r="L24">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="M24" t="s">
         <v>25</v>
@@ -22699,7 +22699,7 @@
         <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F25" t="s">
         <v>24</v>
@@ -22743,16 +22743,16 @@
         <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="H26">
-        <v>2199</v>
+      <c r="H26" t="s">
+        <v>19</v>
       </c>
       <c r="I26" t="s">
         <v>18</v>
@@ -22764,7 +22764,7 @@
         <v>12</v>
       </c>
       <c r="L26">
-        <v>188</v>
+        <v>88</v>
       </c>
       <c r="M26" t="s">
         <v>25</v>
@@ -22787,7 +22787,7 @@
         <v>16</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F27" t="s">
         <v>26</v>
@@ -22831,10 +22831,10 @@
         <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="G28" t="s">
         <v>18</v>
@@ -22872,13 +22872,13 @@
         <v>11377</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="F29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G29" t="s">
         <v>18</v>
@@ -22922,7 +22922,7 @@
         <v>38</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G30" t="s">
         <v>18</v>
@@ -22940,7 +22940,7 @@
         <v>20</v>
       </c>
       <c r="L30">
-        <v>124</v>
+        <v>77</v>
       </c>
       <c r="M30" t="s">
         <v>25</v>
@@ -22963,10 +22963,10 @@
         <v>16</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F31" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G31" t="s">
         <v>18</v>
@@ -22984,7 +22984,7 @@
         <v>1</v>
       </c>
       <c r="L31">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="M31" t="s">
         <v>25</v>
@@ -23010,7 +23010,7 @@
         <v>81</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G32" t="s">
         <v>18</v>
@@ -23051,10 +23051,10 @@
         <v>16</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G33" t="s">
         <v>18</v>
@@ -23072,7 +23072,7 @@
         <v>1</v>
       </c>
       <c r="L33">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="M33" t="s">
         <v>25</v>
@@ -23095,7 +23095,7 @@
         <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="F34" t="s">
         <v>17</v>
@@ -23116,7 +23116,7 @@
         <v>12</v>
       </c>
       <c r="L34">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="M34" t="s">
         <v>25</v>
@@ -23136,10 +23136,10 @@
         <v>11377</v>
       </c>
       <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
         <v>38</v>
-      </c>
-      <c r="E35" t="s">
-        <v>16</v>
       </c>
       <c r="F35" t="s">
         <v>24</v>
@@ -23227,7 +23227,7 @@
         <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="F37" t="s">
         <v>17</v>
@@ -23268,10 +23268,10 @@
         <v>11377</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F38" t="s">
         <v>24</v>
@@ -23312,10 +23312,10 @@
         <v>11377</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="F39" t="s">
         <v>26</v>
@@ -23356,10 +23356,10 @@
         <v>11377</v>
       </c>
       <c r="D40" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F40" t="s">
         <v>17</v>
@@ -23403,7 +23403,7 @@
         <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="F41" t="s">
         <v>24</v>
@@ -23447,10 +23447,10 @@
         <v>16</v>
       </c>
       <c r="E42" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="F42" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G42" t="s">
         <v>18</v>
@@ -23491,7 +23491,7 @@
         <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="F43" t="s">
         <v>17</v>
@@ -23512,7 +23512,7 @@
         <v>10</v>
       </c>
       <c r="L43">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M43" t="s">
         <v>25</v>
@@ -23535,10 +23535,10 @@
         <v>16</v>
       </c>
       <c r="E44" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="F44" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G44" t="s">
         <v>18</v>
@@ -23556,7 +23556,7 @@
         <v>11</v>
       </c>
       <c r="L44">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="M44" t="s">
         <v>25</v>
@@ -23579,7 +23579,7 @@
         <v>16</v>
       </c>
       <c r="E45" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F45" t="s">
         <v>24</v>
@@ -23623,16 +23623,16 @@
         <v>16</v>
       </c>
       <c r="E46" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F46" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G46" t="s">
         <v>18</v>
       </c>
-      <c r="H46">
-        <v>2199</v>
+      <c r="H46" t="s">
+        <v>19</v>
       </c>
       <c r="I46" t="s">
         <v>18</v>
@@ -23644,7 +23644,7 @@
         <v>12</v>
       </c>
       <c r="L46">
-        <v>188</v>
+        <v>88</v>
       </c>
       <c r="M46" t="s">
         <v>25</v>
@@ -23667,7 +23667,7 @@
         <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F47" t="s">
         <v>26</v>
@@ -23711,10 +23711,10 @@
         <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F48" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="G48" t="s">
         <v>18</v>
@@ -23752,13 +23752,13 @@
         <v>11377</v>
       </c>
       <c r="D49" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E49" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="F49" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G49" t="s">
         <v>18</v>
@@ -23802,7 +23802,7 @@
         <v>38</v>
       </c>
       <c r="F50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G50" t="s">
         <v>18</v>
@@ -23820,7 +23820,7 @@
         <v>20</v>
       </c>
       <c r="L50">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="M50" t="s">
         <v>25</v>
@@ -23843,10 +23843,10 @@
         <v>16</v>
       </c>
       <c r="E51" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F51" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G51" t="s">
         <v>18</v>
@@ -23864,7 +23864,7 @@
         <v>1</v>
       </c>
       <c r="L51">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="M51" t="s">
         <v>25</v>

</xml_diff>